<commit_message>
Add change for 'Чек-лист' (demoshopping.ru)
</commit_message>
<xml_diff>
--- a/Test documentation/Checklist/Чек-лист.xlsx
+++ b/Test documentation/Checklist/Чек-лист.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8460" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="9180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1 вариант" sheetId="1" r:id="rId1"/>
@@ -1748,7 +1748,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1888,16 +1888,10 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1905,7 +1899,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1947,9 +1941,6 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1983,26 +1974,11 @@
     <xf numFmtId="0" fontId="6" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2022,41 +1998,12 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -2535,7 +2482,7 @@
   <dimension ref="A1:O967"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="E78" sqref="E78"/>
     </sheetView>
@@ -2577,7 +2524,7 @@
       <c r="L1" s="20"/>
       <c r="M1" s="20"/>
       <c r="N1" s="20"/>
-      <c r="O1" s="63"/>
+      <c r="O1" s="61"/>
     </row>
     <row r="2" ht="16.8" spans="1:15">
       <c r="A2" s="21" t="s">
@@ -2598,7 +2545,7 @@
       <c r="L2" s="25"/>
       <c r="M2" s="25"/>
       <c r="N2" s="25"/>
-      <c r="O2" s="64"/>
+      <c r="O2" s="62"/>
     </row>
     <row r="3" ht="16.8" spans="1:15">
       <c r="A3" s="21" t="s">
@@ -2619,7 +2566,7 @@
       <c r="L3" s="25"/>
       <c r="M3" s="25"/>
       <c r="N3" s="25"/>
-      <c r="O3" s="64"/>
+      <c r="O3" s="62"/>
     </row>
     <row r="4" ht="16.8" spans="1:15">
       <c r="A4" s="21" t="s">
@@ -2640,7 +2587,7 @@
       <c r="L4" s="28"/>
       <c r="M4" s="28"/>
       <c r="N4" s="28"/>
-      <c r="O4" s="65"/>
+      <c r="O4" s="63"/>
     </row>
     <row r="5" ht="50" customHeight="1" spans="1:15">
       <c r="A5" s="29" t="s">
@@ -2669,91 +2616,91 @@
       <c r="N5" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="O5" s="66"/>
+      <c r="O5" s="64"/>
     </row>
     <row r="6" ht="33" customHeight="1" spans="1:15">
-      <c r="A6" s="75" t="s">
+      <c r="A6" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="76" t="s">
+      <c r="B6" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="77" t="s">
+      <c r="C6" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="77" t="s">
+      <c r="D6" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="77" t="s">
+      <c r="E6" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="77" t="s">
+      <c r="F6" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="77" t="s">
+      <c r="G6" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="77" t="s">
+      <c r="H6" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="77" t="s">
+      <c r="I6" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="77" t="s">
+      <c r="J6" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="77" t="s">
+      <c r="K6" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="L6" s="77" t="s">
+      <c r="L6" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="M6" s="77" t="s">
+      <c r="M6" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="N6" s="77" t="s">
+      <c r="N6" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="O6" s="99" t="s">
+      <c r="O6" s="91" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" ht="13.8" spans="1:15">
-      <c r="A7" s="78" t="s">
+      <c r="A7" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="79" t="s">
+      <c r="B7" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="80" t="s">
+      <c r="C7" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="81" t="s">
+      <c r="D7" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="82" t="s">
+      <c r="E7" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="82"/>
-      <c r="K7" s="82"/>
-      <c r="L7" s="82"/>
-      <c r="M7" s="82"/>
-      <c r="N7" s="82"/>
-      <c r="O7" s="100"/>
+      <c r="F7" s="79"/>
+      <c r="G7" s="79"/>
+      <c r="H7" s="79"/>
+      <c r="I7" s="79"/>
+      <c r="J7" s="79"/>
+      <c r="K7" s="79"/>
+      <c r="L7" s="79"/>
+      <c r="M7" s="79"/>
+      <c r="N7" s="79"/>
+      <c r="O7" s="92"/>
     </row>
     <row r="8" ht="27.6" spans="1:15">
       <c r="A8" s="39"/>
       <c r="B8" s="35"/>
-      <c r="C8" s="83"/>
-      <c r="D8" s="84"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="81"/>
       <c r="E8" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="85" t="s">
+      <c r="F8" s="82" t="s">
         <v>26</v>
       </c>
       <c r="G8" s="42"/>
@@ -2764,13 +2711,13 @@
       <c r="L8" s="42"/>
       <c r="M8" s="42"/>
       <c r="N8" s="42"/>
-      <c r="O8" s="69"/>
+      <c r="O8" s="67"/>
     </row>
     <row r="9" ht="27.6" spans="1:15">
       <c r="A9" s="39"/>
       <c r="B9" s="35"/>
-      <c r="C9" s="83"/>
-      <c r="D9" s="84"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="81"/>
       <c r="E9" s="43" t="s">
         <v>27</v>
       </c>
@@ -2785,13 +2732,13 @@
       <c r="L9" s="42"/>
       <c r="M9" s="42"/>
       <c r="N9" s="42"/>
-      <c r="O9" s="69"/>
+      <c r="O9" s="67"/>
     </row>
     <row r="10" ht="27.6" spans="1:15">
       <c r="A10" s="39"/>
       <c r="B10" s="35"/>
-      <c r="C10" s="83"/>
-      <c r="D10" s="84"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="81"/>
       <c r="E10" s="43" t="s">
         <v>29</v>
       </c>
@@ -2804,13 +2751,13 @@
       <c r="L10" s="42"/>
       <c r="M10" s="42"/>
       <c r="N10" s="42"/>
-      <c r="O10" s="69"/>
+      <c r="O10" s="67"/>
     </row>
     <row r="11" ht="27.6" spans="1:15">
       <c r="A11" s="39"/>
       <c r="B11" s="35"/>
-      <c r="C11" s="83"/>
-      <c r="D11" s="84"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="81"/>
       <c r="E11" s="43" t="s">
         <v>30</v>
       </c>
@@ -2823,32 +2770,32 @@
       <c r="L11" s="42"/>
       <c r="M11" s="42"/>
       <c r="N11" s="42"/>
-      <c r="O11" s="69"/>
+      <c r="O11" s="67"/>
     </row>
     <row r="12" ht="13.8" spans="1:15">
       <c r="A12" s="39"/>
       <c r="B12" s="35"/>
-      <c r="C12" s="83"/>
-      <c r="D12" s="84"/>
-      <c r="E12" s="86" t="s">
+      <c r="C12" s="80"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="83" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="86"/>
-      <c r="G12" s="86"/>
-      <c r="H12" s="86"/>
-      <c r="I12" s="86"/>
-      <c r="J12" s="86"/>
-      <c r="K12" s="86"/>
-      <c r="L12" s="86"/>
-      <c r="M12" s="86"/>
-      <c r="N12" s="86"/>
-      <c r="O12" s="101"/>
+      <c r="F12" s="83"/>
+      <c r="G12" s="83"/>
+      <c r="H12" s="83"/>
+      <c r="I12" s="83"/>
+      <c r="J12" s="83"/>
+      <c r="K12" s="83"/>
+      <c r="L12" s="83"/>
+      <c r="M12" s="83"/>
+      <c r="N12" s="83"/>
+      <c r="O12" s="93"/>
     </row>
     <row r="13" ht="13.8" spans="1:15">
       <c r="A13" s="39"/>
       <c r="B13" s="35"/>
-      <c r="C13" s="83"/>
-      <c r="D13" s="84"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="81"/>
       <c r="E13" s="43" t="s">
         <v>32</v>
       </c>
@@ -2861,13 +2808,13 @@
       <c r="L13" s="42"/>
       <c r="M13" s="42"/>
       <c r="N13" s="42"/>
-      <c r="O13" s="69"/>
+      <c r="O13" s="67"/>
     </row>
     <row r="14" ht="27.6" spans="1:15">
       <c r="A14" s="39"/>
       <c r="B14" s="35"/>
-      <c r="C14" s="83"/>
-      <c r="D14" s="84"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="81"/>
       <c r="E14" s="43" t="s">
         <v>33</v>
       </c>
@@ -2880,13 +2827,13 @@
       <c r="L14" s="42"/>
       <c r="M14" s="42"/>
       <c r="N14" s="42"/>
-      <c r="O14" s="69"/>
+      <c r="O14" s="67"/>
     </row>
     <row r="15" ht="27.6" spans="1:15">
       <c r="A15" s="39"/>
       <c r="B15" s="35"/>
-      <c r="C15" s="83"/>
-      <c r="D15" s="84"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="81"/>
       <c r="E15" s="43" t="s">
         <v>34</v>
       </c>
@@ -2899,13 +2846,13 @@
       <c r="L15" s="42"/>
       <c r="M15" s="42"/>
       <c r="N15" s="42"/>
-      <c r="O15" s="69"/>
+      <c r="O15" s="67"/>
     </row>
     <row r="16" ht="27.6" spans="1:15">
       <c r="A16" s="39"/>
       <c r="B16" s="35"/>
-      <c r="C16" s="83"/>
-      <c r="D16" s="84"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="81"/>
       <c r="E16" s="43" t="s">
         <v>35</v>
       </c>
@@ -2918,13 +2865,13 @@
       <c r="L16" s="42"/>
       <c r="M16" s="42"/>
       <c r="N16" s="42"/>
-      <c r="O16" s="69"/>
+      <c r="O16" s="67"/>
     </row>
     <row r="17" ht="27.6" spans="1:15">
       <c r="A17" s="39"/>
       <c r="B17" s="35"/>
-      <c r="C17" s="83"/>
-      <c r="D17" s="84"/>
+      <c r="C17" s="80"/>
+      <c r="D17" s="81"/>
       <c r="E17" s="43" t="s">
         <v>36</v>
       </c>
@@ -2937,13 +2884,13 @@
       <c r="L17" s="42"/>
       <c r="M17" s="42"/>
       <c r="N17" s="42"/>
-      <c r="O17" s="69"/>
+      <c r="O17" s="67"/>
     </row>
     <row r="18" ht="13.8" spans="1:15">
       <c r="A18" s="39"/>
       <c r="B18" s="35"/>
-      <c r="C18" s="83"/>
-      <c r="D18" s="84"/>
+      <c r="C18" s="80"/>
+      <c r="D18" s="81"/>
       <c r="E18" s="43" t="s">
         <v>37</v>
       </c>
@@ -2956,13 +2903,13 @@
       <c r="L18" s="42"/>
       <c r="M18" s="42"/>
       <c r="N18" s="42"/>
-      <c r="O18" s="69"/>
+      <c r="O18" s="67"/>
     </row>
     <row r="19" ht="13.8" spans="1:15">
       <c r="A19" s="39"/>
       <c r="B19" s="35"/>
-      <c r="C19" s="83"/>
-      <c r="D19" s="84"/>
+      <c r="C19" s="80"/>
+      <c r="D19" s="81"/>
       <c r="E19" s="43" t="s">
         <v>38</v>
       </c>
@@ -2975,978 +2922,978 @@
       <c r="L19" s="42"/>
       <c r="M19" s="42"/>
       <c r="N19" s="42"/>
-      <c r="O19" s="69"/>
+      <c r="O19" s="67"/>
     </row>
     <row r="20" ht="13.8" spans="1:15">
       <c r="A20" s="39"/>
       <c r="B20" s="35"/>
-      <c r="C20" s="83"/>
-      <c r="D20" s="84" t="s">
+      <c r="C20" s="80"/>
+      <c r="D20" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="E20" s="87" t="s">
+      <c r="E20" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="87"/>
-      <c r="G20" s="87"/>
-      <c r="H20" s="87"/>
-      <c r="I20" s="87"/>
-      <c r="J20" s="87"/>
-      <c r="K20" s="87"/>
-      <c r="L20" s="87"/>
-      <c r="M20" s="87"/>
-      <c r="N20" s="87"/>
-      <c r="O20" s="102"/>
+      <c r="F20" s="84"/>
+      <c r="G20" s="84"/>
+      <c r="H20" s="84"/>
+      <c r="I20" s="84"/>
+      <c r="J20" s="84"/>
+      <c r="K20" s="84"/>
+      <c r="L20" s="84"/>
+      <c r="M20" s="84"/>
+      <c r="N20" s="84"/>
+      <c r="O20" s="94"/>
     </row>
     <row r="21" ht="27.6" spans="1:15">
       <c r="A21" s="39"/>
       <c r="B21" s="35"/>
-      <c r="C21" s="83"/>
-      <c r="D21" s="84"/>
+      <c r="C21" s="80"/>
+      <c r="D21" s="81"/>
       <c r="E21" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="F21" s="53"/>
-      <c r="G21" s="53"/>
-      <c r="H21" s="53"/>
-      <c r="I21" s="53"/>
-      <c r="J21" s="53"/>
-      <c r="K21" s="53"/>
-      <c r="L21" s="53"/>
-      <c r="M21" s="53"/>
-      <c r="N21" s="53"/>
-      <c r="O21" s="72"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="52"/>
+      <c r="I21" s="52"/>
+      <c r="J21" s="52"/>
+      <c r="K21" s="52"/>
+      <c r="L21" s="52"/>
+      <c r="M21" s="52"/>
+      <c r="N21" s="52"/>
+      <c r="O21" s="70"/>
     </row>
     <row r="22" ht="27.6" spans="1:15">
       <c r="A22" s="39"/>
       <c r="B22" s="35"/>
-      <c r="C22" s="83"/>
-      <c r="D22" s="84"/>
+      <c r="C22" s="80"/>
+      <c r="D22" s="81"/>
       <c r="E22" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="F22" s="53"/>
-      <c r="G22" s="53"/>
-      <c r="H22" s="53"/>
-      <c r="I22" s="53"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="53"/>
-      <c r="L22" s="53"/>
-      <c r="M22" s="53"/>
-      <c r="N22" s="53"/>
-      <c r="O22" s="72"/>
+      <c r="F22" s="52"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="52"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="52"/>
+      <c r="K22" s="52"/>
+      <c r="L22" s="52"/>
+      <c r="M22" s="52"/>
+      <c r="N22" s="52"/>
+      <c r="O22" s="70"/>
     </row>
     <row r="23" ht="13.8" spans="1:15">
       <c r="A23" s="39"/>
       <c r="B23" s="35"/>
-      <c r="C23" s="83"/>
-      <c r="D23" s="84"/>
-      <c r="E23" s="86" t="s">
+      <c r="C23" s="80"/>
+      <c r="D23" s="81"/>
+      <c r="E23" s="83" t="s">
         <v>31</v>
       </c>
-      <c r="F23" s="86"/>
-      <c r="G23" s="86"/>
-      <c r="H23" s="86"/>
-      <c r="I23" s="86"/>
-      <c r="J23" s="86"/>
-      <c r="K23" s="86"/>
-      <c r="L23" s="86"/>
-      <c r="M23" s="86"/>
-      <c r="N23" s="86"/>
-      <c r="O23" s="101"/>
+      <c r="F23" s="83"/>
+      <c r="G23" s="83"/>
+      <c r="H23" s="83"/>
+      <c r="I23" s="83"/>
+      <c r="J23" s="83"/>
+      <c r="K23" s="83"/>
+      <c r="L23" s="83"/>
+      <c r="M23" s="83"/>
+      <c r="N23" s="83"/>
+      <c r="O23" s="93"/>
     </row>
     <row r="24" ht="13.8" spans="1:15">
       <c r="A24" s="39"/>
       <c r="B24" s="35"/>
-      <c r="C24" s="83"/>
-      <c r="D24" s="84"/>
+      <c r="C24" s="80"/>
+      <c r="D24" s="81"/>
       <c r="E24" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="F24" s="53"/>
-      <c r="G24" s="53"/>
-      <c r="H24" s="53"/>
-      <c r="I24" s="53"/>
-      <c r="J24" s="53"/>
-      <c r="K24" s="53"/>
-      <c r="L24" s="53"/>
-      <c r="M24" s="53"/>
-      <c r="N24" s="53"/>
-      <c r="O24" s="72"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="52"/>
+      <c r="L24" s="52"/>
+      <c r="M24" s="52"/>
+      <c r="N24" s="52"/>
+      <c r="O24" s="70"/>
     </row>
     <row r="25" ht="27.6" spans="1:15">
       <c r="A25" s="39"/>
       <c r="B25" s="35"/>
-      <c r="C25" s="83"/>
-      <c r="D25" s="84"/>
+      <c r="C25" s="80"/>
+      <c r="D25" s="81"/>
       <c r="E25" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="F25" s="53"/>
-      <c r="G25" s="53"/>
-      <c r="H25" s="53"/>
-      <c r="I25" s="53"/>
-      <c r="J25" s="53"/>
-      <c r="K25" s="53"/>
-      <c r="L25" s="53"/>
-      <c r="M25" s="53"/>
-      <c r="N25" s="53"/>
-      <c r="O25" s="72"/>
+      <c r="F25" s="52"/>
+      <c r="G25" s="52"/>
+      <c r="H25" s="52"/>
+      <c r="I25" s="52"/>
+      <c r="J25" s="52"/>
+      <c r="K25" s="52"/>
+      <c r="L25" s="52"/>
+      <c r="M25" s="52"/>
+      <c r="N25" s="52"/>
+      <c r="O25" s="70"/>
     </row>
     <row r="26" ht="27.6" spans="1:15">
       <c r="A26" s="39"/>
       <c r="B26" s="35"/>
-      <c r="C26" s="83"/>
-      <c r="D26" s="84"/>
+      <c r="C26" s="80"/>
+      <c r="D26" s="81"/>
       <c r="E26" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="F26" s="53"/>
-      <c r="G26" s="53"/>
-      <c r="H26" s="53"/>
-      <c r="I26" s="53"/>
-      <c r="J26" s="53"/>
-      <c r="K26" s="53"/>
-      <c r="L26" s="53"/>
-      <c r="M26" s="53"/>
-      <c r="N26" s="53"/>
-      <c r="O26" s="72"/>
+      <c r="F26" s="52"/>
+      <c r="G26" s="52"/>
+      <c r="H26" s="52"/>
+      <c r="I26" s="52"/>
+      <c r="J26" s="52"/>
+      <c r="K26" s="52"/>
+      <c r="L26" s="52"/>
+      <c r="M26" s="52"/>
+      <c r="N26" s="52"/>
+      <c r="O26" s="70"/>
     </row>
     <row r="27" ht="27.6" spans="1:15">
       <c r="A27" s="39"/>
       <c r="B27" s="35"/>
-      <c r="C27" s="83"/>
-      <c r="D27" s="84"/>
+      <c r="C27" s="80"/>
+      <c r="D27" s="81"/>
       <c r="E27" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="53"/>
-      <c r="G27" s="53"/>
-      <c r="H27" s="53"/>
-      <c r="I27" s="53"/>
-      <c r="J27" s="53"/>
-      <c r="K27" s="53"/>
-      <c r="L27" s="53"/>
-      <c r="M27" s="53"/>
-      <c r="N27" s="53"/>
-      <c r="O27" s="72"/>
+      <c r="F27" s="52"/>
+      <c r="G27" s="52"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="52"/>
+      <c r="J27" s="52"/>
+      <c r="K27" s="52"/>
+      <c r="L27" s="52"/>
+      <c r="M27" s="52"/>
+      <c r="N27" s="52"/>
+      <c r="O27" s="70"/>
     </row>
     <row r="28" ht="13.8" spans="1:15">
       <c r="A28" s="39"/>
       <c r="B28" s="35"/>
-      <c r="C28" s="83"/>
-      <c r="D28" s="84"/>
+      <c r="C28" s="80"/>
+      <c r="D28" s="81"/>
       <c r="E28" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="F28" s="53"/>
-      <c r="G28" s="53"/>
-      <c r="H28" s="53"/>
-      <c r="I28" s="53"/>
-      <c r="J28" s="53"/>
-      <c r="K28" s="53"/>
-      <c r="L28" s="53"/>
-      <c r="M28" s="53"/>
-      <c r="N28" s="53"/>
-      <c r="O28" s="72"/>
+      <c r="F28" s="52"/>
+      <c r="G28" s="52"/>
+      <c r="H28" s="52"/>
+      <c r="I28" s="52"/>
+      <c r="J28" s="52"/>
+      <c r="K28" s="52"/>
+      <c r="L28" s="52"/>
+      <c r="M28" s="52"/>
+      <c r="N28" s="52"/>
+      <c r="O28" s="70"/>
     </row>
     <row r="29" ht="13.8" spans="1:15">
       <c r="A29" s="39"/>
       <c r="B29" s="35"/>
-      <c r="C29" s="83"/>
-      <c r="D29" s="84"/>
+      <c r="C29" s="80"/>
+      <c r="D29" s="81"/>
       <c r="E29" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="F29" s="53"/>
-      <c r="G29" s="53"/>
-      <c r="H29" s="53"/>
-      <c r="I29" s="53"/>
-      <c r="J29" s="53"/>
-      <c r="K29" s="53"/>
-      <c r="L29" s="53"/>
-      <c r="M29" s="53"/>
-      <c r="N29" s="53"/>
-      <c r="O29" s="72"/>
+      <c r="F29" s="52"/>
+      <c r="G29" s="52"/>
+      <c r="H29" s="52"/>
+      <c r="I29" s="52"/>
+      <c r="J29" s="52"/>
+      <c r="K29" s="52"/>
+      <c r="L29" s="52"/>
+      <c r="M29" s="52"/>
+      <c r="N29" s="52"/>
+      <c r="O29" s="70"/>
     </row>
     <row r="30" ht="13.8" spans="1:15">
       <c r="A30" s="39"/>
       <c r="B30" s="35"/>
-      <c r="C30" s="83"/>
-      <c r="D30" s="84"/>
+      <c r="C30" s="80"/>
+      <c r="D30" s="81"/>
       <c r="E30" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="F30" s="53"/>
-      <c r="G30" s="53"/>
-      <c r="H30" s="53"/>
-      <c r="I30" s="53"/>
-      <c r="J30" s="53"/>
-      <c r="K30" s="53"/>
-      <c r="L30" s="53"/>
-      <c r="M30" s="53"/>
-      <c r="N30" s="53"/>
-      <c r="O30" s="72"/>
+      <c r="F30" s="52"/>
+      <c r="G30" s="52"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="52"/>
+      <c r="J30" s="52"/>
+      <c r="K30" s="52"/>
+      <c r="L30" s="52"/>
+      <c r="M30" s="52"/>
+      <c r="N30" s="52"/>
+      <c r="O30" s="70"/>
     </row>
     <row r="31" ht="14.55" spans="1:15">
       <c r="A31" s="44"/>
       <c r="B31" s="35"/>
-      <c r="C31" s="88"/>
-      <c r="D31" s="89"/>
+      <c r="C31" s="85"/>
+      <c r="D31" s="86"/>
       <c r="E31" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="F31" s="56"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="56"/>
-      <c r="J31" s="56"/>
-      <c r="K31" s="56"/>
-      <c r="L31" s="56"/>
-      <c r="M31" s="56"/>
-      <c r="N31" s="56"/>
-      <c r="O31" s="73"/>
+      <c r="F31" s="54"/>
+      <c r="G31" s="54"/>
+      <c r="H31" s="54"/>
+      <c r="I31" s="54"/>
+      <c r="J31" s="54"/>
+      <c r="K31" s="54"/>
+      <c r="L31" s="54"/>
+      <c r="M31" s="54"/>
+      <c r="N31" s="54"/>
+      <c r="O31" s="71"/>
     </row>
     <row r="32" ht="13.8" spans="1:15">
-      <c r="A32" s="78" t="s">
+      <c r="A32" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="B32" s="90" t="s">
+      <c r="B32" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="80" t="s">
+      <c r="C32" s="77" t="s">
         <v>50</v>
       </c>
-      <c r="D32" s="81" t="s">
+      <c r="D32" s="78" t="s">
         <v>51</v>
       </c>
-      <c r="E32" s="82" t="s">
+      <c r="E32" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="F32" s="82"/>
-      <c r="G32" s="82"/>
-      <c r="H32" s="82"/>
-      <c r="I32" s="82"/>
-      <c r="J32" s="82"/>
-      <c r="K32" s="82"/>
-      <c r="L32" s="82"/>
-      <c r="M32" s="82"/>
-      <c r="N32" s="82"/>
-      <c r="O32" s="100"/>
+      <c r="F32" s="79"/>
+      <c r="G32" s="79"/>
+      <c r="H32" s="79"/>
+      <c r="I32" s="79"/>
+      <c r="J32" s="79"/>
+      <c r="K32" s="79"/>
+      <c r="L32" s="79"/>
+      <c r="M32" s="79"/>
+      <c r="N32" s="79"/>
+      <c r="O32" s="92"/>
     </row>
     <row r="33" ht="13.8" spans="1:15">
       <c r="A33" s="39"/>
-      <c r="B33" s="91"/>
-      <c r="C33" s="83"/>
-      <c r="D33" s="84"/>
+      <c r="B33" s="51"/>
+      <c r="C33" s="80"/>
+      <c r="D33" s="81"/>
       <c r="E33" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="F33" s="53"/>
-      <c r="G33" s="53"/>
-      <c r="H33" s="53"/>
-      <c r="I33" s="53"/>
-      <c r="J33" s="53"/>
-      <c r="K33" s="53"/>
-      <c r="L33" s="53"/>
-      <c r="M33" s="53"/>
-      <c r="N33" s="53"/>
-      <c r="O33" s="72"/>
+      <c r="F33" s="52"/>
+      <c r="G33" s="52"/>
+      <c r="H33" s="52"/>
+      <c r="I33" s="52"/>
+      <c r="J33" s="52"/>
+      <c r="K33" s="52"/>
+      <c r="L33" s="52"/>
+      <c r="M33" s="52"/>
+      <c r="N33" s="52"/>
+      <c r="O33" s="70"/>
     </row>
     <row r="34" ht="13.8" spans="1:15">
       <c r="A34" s="39"/>
-      <c r="B34" s="91"/>
-      <c r="C34" s="83"/>
-      <c r="D34" s="84"/>
-      <c r="E34" s="86" t="s">
+      <c r="B34" s="51"/>
+      <c r="C34" s="80"/>
+      <c r="D34" s="81"/>
+      <c r="E34" s="83" t="s">
         <v>31</v>
       </c>
-      <c r="F34" s="86"/>
-      <c r="G34" s="86"/>
-      <c r="H34" s="86"/>
-      <c r="I34" s="86"/>
-      <c r="J34" s="86"/>
-      <c r="K34" s="86"/>
-      <c r="L34" s="86"/>
-      <c r="M34" s="86"/>
-      <c r="N34" s="86"/>
-      <c r="O34" s="101"/>
+      <c r="F34" s="83"/>
+      <c r="G34" s="83"/>
+      <c r="H34" s="83"/>
+      <c r="I34" s="83"/>
+      <c r="J34" s="83"/>
+      <c r="K34" s="83"/>
+      <c r="L34" s="83"/>
+      <c r="M34" s="83"/>
+      <c r="N34" s="83"/>
+      <c r="O34" s="93"/>
     </row>
     <row r="35" ht="13.8" spans="1:15">
       <c r="A35" s="39"/>
-      <c r="B35" s="91"/>
-      <c r="C35" s="83"/>
-      <c r="D35" s="84"/>
+      <c r="B35" s="51"/>
+      <c r="C35" s="80"/>
+      <c r="D35" s="81"/>
       <c r="E35" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="F35" s="53"/>
-      <c r="G35" s="53"/>
-      <c r="H35" s="53"/>
-      <c r="I35" s="53"/>
-      <c r="J35" s="53"/>
-      <c r="K35" s="53"/>
-      <c r="L35" s="53"/>
-      <c r="M35" s="53"/>
-      <c r="N35" s="53"/>
-      <c r="O35" s="72"/>
+      <c r="F35" s="52"/>
+      <c r="G35" s="52"/>
+      <c r="H35" s="52"/>
+      <c r="I35" s="52"/>
+      <c r="J35" s="52"/>
+      <c r="K35" s="52"/>
+      <c r="L35" s="52"/>
+      <c r="M35" s="52"/>
+      <c r="N35" s="52"/>
+      <c r="O35" s="70"/>
     </row>
     <row r="36" ht="13.8" spans="1:15">
       <c r="A36" s="39"/>
-      <c r="B36" s="91"/>
-      <c r="C36" s="83"/>
-      <c r="D36" s="84"/>
+      <c r="B36" s="51"/>
+      <c r="C36" s="80"/>
+      <c r="D36" s="81"/>
       <c r="E36" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="F36" s="53"/>
-      <c r="G36" s="53"/>
-      <c r="H36" s="53"/>
-      <c r="I36" s="53"/>
-      <c r="J36" s="53"/>
-      <c r="K36" s="53"/>
-      <c r="L36" s="53"/>
-      <c r="M36" s="53"/>
-      <c r="N36" s="53"/>
-      <c r="O36" s="72"/>
+      <c r="F36" s="52"/>
+      <c r="G36" s="52"/>
+      <c r="H36" s="52"/>
+      <c r="I36" s="52"/>
+      <c r="J36" s="52"/>
+      <c r="K36" s="52"/>
+      <c r="L36" s="52"/>
+      <c r="M36" s="52"/>
+      <c r="N36" s="52"/>
+      <c r="O36" s="70"/>
     </row>
     <row r="37" ht="13.8" spans="1:15">
       <c r="A37" s="39"/>
-      <c r="B37" s="91"/>
-      <c r="C37" s="83"/>
-      <c r="D37" s="84"/>
+      <c r="B37" s="51"/>
+      <c r="C37" s="80"/>
+      <c r="D37" s="81"/>
       <c r="E37" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="F37" s="53"/>
-      <c r="G37" s="53"/>
-      <c r="H37" s="53"/>
-      <c r="I37" s="53"/>
-      <c r="J37" s="53"/>
-      <c r="K37" s="53"/>
-      <c r="L37" s="53"/>
-      <c r="M37" s="53"/>
-      <c r="N37" s="53"/>
-      <c r="O37" s="72"/>
+      <c r="F37" s="52"/>
+      <c r="G37" s="52"/>
+      <c r="H37" s="52"/>
+      <c r="I37" s="52"/>
+      <c r="J37" s="52"/>
+      <c r="K37" s="52"/>
+      <c r="L37" s="52"/>
+      <c r="M37" s="52"/>
+      <c r="N37" s="52"/>
+      <c r="O37" s="70"/>
     </row>
     <row r="38" ht="14.55" spans="1:15">
-      <c r="A38" s="92"/>
-      <c r="B38" s="93"/>
-      <c r="C38" s="94"/>
-      <c r="D38" s="95"/>
-      <c r="E38" s="61" t="s">
+      <c r="A38" s="57"/>
+      <c r="B38" s="58"/>
+      <c r="C38" s="87"/>
+      <c r="D38" s="88"/>
+      <c r="E38" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="F38" s="62"/>
-      <c r="G38" s="62"/>
-      <c r="H38" s="62"/>
-      <c r="I38" s="62"/>
-      <c r="J38" s="62"/>
-      <c r="K38" s="62"/>
-      <c r="L38" s="62"/>
-      <c r="M38" s="62"/>
-      <c r="N38" s="62"/>
-      <c r="O38" s="74"/>
+      <c r="F38" s="60"/>
+      <c r="G38" s="60"/>
+      <c r="H38" s="60"/>
+      <c r="I38" s="60"/>
+      <c r="J38" s="60"/>
+      <c r="K38" s="60"/>
+      <c r="L38" s="60"/>
+      <c r="M38" s="60"/>
+      <c r="N38" s="60"/>
+      <c r="O38" s="72"/>
     </row>
     <row r="39" ht="13.8" spans="1:15">
-      <c r="A39" s="78" t="s">
+      <c r="A39" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="B39" s="90" t="s">
+      <c r="B39" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="C39" s="80" t="s">
+      <c r="C39" s="77" t="s">
         <v>59</v>
       </c>
-      <c r="D39" s="81" t="s">
+      <c r="D39" s="78" t="s">
         <v>60</v>
       </c>
-      <c r="E39" s="82" t="s">
+      <c r="E39" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="F39" s="82"/>
-      <c r="G39" s="82"/>
-      <c r="H39" s="82"/>
-      <c r="I39" s="82"/>
-      <c r="J39" s="82"/>
-      <c r="K39" s="82"/>
-      <c r="L39" s="82"/>
-      <c r="M39" s="82"/>
-      <c r="N39" s="82"/>
-      <c r="O39" s="100"/>
+      <c r="F39" s="79"/>
+      <c r="G39" s="79"/>
+      <c r="H39" s="79"/>
+      <c r="I39" s="79"/>
+      <c r="J39" s="79"/>
+      <c r="K39" s="79"/>
+      <c r="L39" s="79"/>
+      <c r="M39" s="79"/>
+      <c r="N39" s="79"/>
+      <c r="O39" s="92"/>
     </row>
     <row r="40" ht="24" customHeight="1" spans="1:15">
       <c r="A40" s="39"/>
-      <c r="B40" s="91"/>
-      <c r="C40" s="83"/>
-      <c r="D40" s="84"/>
+      <c r="B40" s="51"/>
+      <c r="C40" s="80"/>
+      <c r="D40" s="81"/>
       <c r="E40" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="F40" s="53"/>
-      <c r="G40" s="53"/>
-      <c r="H40" s="53"/>
-      <c r="I40" s="53"/>
-      <c r="J40" s="53"/>
-      <c r="K40" s="53"/>
-      <c r="L40" s="53"/>
-      <c r="M40" s="53"/>
-      <c r="N40" s="53"/>
-      <c r="O40" s="72"/>
+      <c r="F40" s="52"/>
+      <c r="G40" s="52"/>
+      <c r="H40" s="52"/>
+      <c r="I40" s="52"/>
+      <c r="J40" s="52"/>
+      <c r="K40" s="52"/>
+      <c r="L40" s="52"/>
+      <c r="M40" s="52"/>
+      <c r="N40" s="52"/>
+      <c r="O40" s="70"/>
     </row>
     <row r="41" ht="36" customHeight="1" spans="1:15">
       <c r="A41" s="39"/>
-      <c r="B41" s="91"/>
-      <c r="C41" s="83"/>
-      <c r="D41" s="84"/>
+      <c r="B41" s="51"/>
+      <c r="C41" s="80"/>
+      <c r="D41" s="81"/>
       <c r="E41" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="F41" s="53"/>
-      <c r="G41" s="53"/>
-      <c r="H41" s="53"/>
-      <c r="I41" s="53"/>
-      <c r="J41" s="53"/>
-      <c r="K41" s="53"/>
-      <c r="L41" s="53"/>
-      <c r="M41" s="53"/>
-      <c r="N41" s="53"/>
-      <c r="O41" s="72"/>
+      <c r="F41" s="52"/>
+      <c r="G41" s="52"/>
+      <c r="H41" s="52"/>
+      <c r="I41" s="52"/>
+      <c r="J41" s="52"/>
+      <c r="K41" s="52"/>
+      <c r="L41" s="52"/>
+      <c r="M41" s="52"/>
+      <c r="N41" s="52"/>
+      <c r="O41" s="70"/>
     </row>
     <row r="42" ht="49" customHeight="1" spans="1:15">
       <c r="A42" s="39"/>
-      <c r="B42" s="91"/>
-      <c r="C42" s="83"/>
-      <c r="D42" s="84"/>
+      <c r="B42" s="51"/>
+      <c r="C42" s="80"/>
+      <c r="D42" s="81"/>
       <c r="E42" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="F42" s="53"/>
-      <c r="G42" s="53"/>
-      <c r="H42" s="53"/>
-      <c r="I42" s="53"/>
-      <c r="J42" s="53"/>
-      <c r="K42" s="53"/>
-      <c r="L42" s="53"/>
-      <c r="M42" s="53"/>
-      <c r="N42" s="53"/>
-      <c r="O42" s="72"/>
+      <c r="F42" s="52"/>
+      <c r="G42" s="52"/>
+      <c r="H42" s="52"/>
+      <c r="I42" s="52"/>
+      <c r="J42" s="52"/>
+      <c r="K42" s="52"/>
+      <c r="L42" s="52"/>
+      <c r="M42" s="52"/>
+      <c r="N42" s="52"/>
+      <c r="O42" s="70"/>
     </row>
     <row r="43" ht="49" customHeight="1" spans="1:15">
       <c r="A43" s="39"/>
-      <c r="B43" s="91"/>
-      <c r="C43" s="83"/>
-      <c r="D43" s="84"/>
+      <c r="B43" s="51"/>
+      <c r="C43" s="80"/>
+      <c r="D43" s="81"/>
       <c r="E43" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="F43" s="53"/>
-      <c r="G43" s="53"/>
-      <c r="H43" s="53"/>
-      <c r="I43" s="53"/>
-      <c r="J43" s="53"/>
-      <c r="K43" s="53"/>
-      <c r="L43" s="53"/>
-      <c r="M43" s="53"/>
-      <c r="N43" s="53"/>
-      <c r="O43" s="72"/>
+      <c r="F43" s="52"/>
+      <c r="G43" s="52"/>
+      <c r="H43" s="52"/>
+      <c r="I43" s="52"/>
+      <c r="J43" s="52"/>
+      <c r="K43" s="52"/>
+      <c r="L43" s="52"/>
+      <c r="M43" s="52"/>
+      <c r="N43" s="52"/>
+      <c r="O43" s="70"/>
     </row>
     <row r="44" ht="39" customHeight="1" spans="1:15">
       <c r="A44" s="39"/>
-      <c r="B44" s="91"/>
-      <c r="C44" s="83"/>
-      <c r="D44" s="84"/>
+      <c r="B44" s="51"/>
+      <c r="C44" s="80"/>
+      <c r="D44" s="81"/>
       <c r="E44" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="F44" s="53"/>
-      <c r="G44" s="53"/>
-      <c r="H44" s="53"/>
-      <c r="I44" s="53"/>
-      <c r="J44" s="53"/>
-      <c r="K44" s="53"/>
-      <c r="L44" s="53"/>
-      <c r="M44" s="53"/>
-      <c r="N44" s="53"/>
-      <c r="O44" s="72"/>
+      <c r="F44" s="52"/>
+      <c r="G44" s="52"/>
+      <c r="H44" s="52"/>
+      <c r="I44" s="52"/>
+      <c r="J44" s="52"/>
+      <c r="K44" s="52"/>
+      <c r="L44" s="52"/>
+      <c r="M44" s="52"/>
+      <c r="N44" s="52"/>
+      <c r="O44" s="70"/>
     </row>
     <row r="45" ht="35" customHeight="1" spans="1:15">
       <c r="A45" s="44"/>
-      <c r="B45" s="96"/>
-      <c r="C45" s="88"/>
-      <c r="D45" s="89"/>
+      <c r="B45" s="53"/>
+      <c r="C45" s="85"/>
+      <c r="D45" s="86"/>
       <c r="E45" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="F45" s="56"/>
-      <c r="G45" s="56"/>
-      <c r="H45" s="56"/>
-      <c r="I45" s="56"/>
-      <c r="J45" s="56"/>
-      <c r="K45" s="56"/>
-      <c r="L45" s="56"/>
-      <c r="M45" s="56"/>
-      <c r="N45" s="56"/>
-      <c r="O45" s="73"/>
+      <c r="F45" s="54"/>
+      <c r="G45" s="54"/>
+      <c r="H45" s="54"/>
+      <c r="I45" s="54"/>
+      <c r="J45" s="54"/>
+      <c r="K45" s="54"/>
+      <c r="L45" s="54"/>
+      <c r="M45" s="54"/>
+      <c r="N45" s="54"/>
+      <c r="O45" s="71"/>
     </row>
     <row r="46" ht="15" customHeight="1" spans="1:15">
-      <c r="A46" s="78" t="s">
+      <c r="A46" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="B46" s="90" t="s">
+      <c r="B46" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="80" t="s">
+      <c r="C46" s="77" t="s">
         <v>68</v>
       </c>
-      <c r="D46" s="81" t="s">
+      <c r="D46" s="78" t="s">
         <v>69</v>
       </c>
-      <c r="E46" s="82" t="s">
+      <c r="E46" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="F46" s="82"/>
-      <c r="G46" s="82"/>
-      <c r="H46" s="82"/>
-      <c r="I46" s="82"/>
-      <c r="J46" s="82"/>
-      <c r="K46" s="82"/>
-      <c r="L46" s="82"/>
-      <c r="M46" s="82"/>
-      <c r="N46" s="82"/>
-      <c r="O46" s="100"/>
+      <c r="F46" s="79"/>
+      <c r="G46" s="79"/>
+      <c r="H46" s="79"/>
+      <c r="I46" s="79"/>
+      <c r="J46" s="79"/>
+      <c r="K46" s="79"/>
+      <c r="L46" s="79"/>
+      <c r="M46" s="79"/>
+      <c r="N46" s="79"/>
+      <c r="O46" s="92"/>
     </row>
     <row r="47" ht="27" customHeight="1" spans="1:15">
       <c r="A47" s="39"/>
-      <c r="B47" s="91"/>
-      <c r="C47" s="83"/>
-      <c r="D47" s="84"/>
+      <c r="B47" s="51"/>
+      <c r="C47" s="80"/>
+      <c r="D47" s="81"/>
       <c r="E47" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="F47" s="53"/>
-      <c r="G47" s="53"/>
-      <c r="H47" s="53"/>
-      <c r="I47" s="53"/>
-      <c r="J47" s="53"/>
-      <c r="K47" s="53"/>
-      <c r="L47" s="53"/>
-      <c r="M47" s="53"/>
-      <c r="N47" s="53"/>
-      <c r="O47" s="72"/>
+      <c r="F47" s="52"/>
+      <c r="G47" s="52"/>
+      <c r="H47" s="52"/>
+      <c r="I47" s="52"/>
+      <c r="J47" s="52"/>
+      <c r="K47" s="52"/>
+      <c r="L47" s="52"/>
+      <c r="M47" s="52"/>
+      <c r="N47" s="52"/>
+      <c r="O47" s="70"/>
     </row>
     <row r="48" ht="25" customHeight="1" spans="1:15">
       <c r="A48" s="39"/>
-      <c r="B48" s="91"/>
-      <c r="C48" s="83"/>
-      <c r="D48" s="84"/>
+      <c r="B48" s="51"/>
+      <c r="C48" s="80"/>
+      <c r="D48" s="81"/>
       <c r="E48" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="F48" s="53"/>
-      <c r="G48" s="53"/>
-      <c r="H48" s="53"/>
-      <c r="I48" s="53"/>
-      <c r="J48" s="53"/>
-      <c r="K48" s="53"/>
-      <c r="L48" s="53"/>
-      <c r="M48" s="53"/>
-      <c r="N48" s="53"/>
-      <c r="O48" s="72"/>
+      <c r="F48" s="52"/>
+      <c r="G48" s="52"/>
+      <c r="H48" s="52"/>
+      <c r="I48" s="52"/>
+      <c r="J48" s="52"/>
+      <c r="K48" s="52"/>
+      <c r="L48" s="52"/>
+      <c r="M48" s="52"/>
+      <c r="N48" s="52"/>
+      <c r="O48" s="70"/>
     </row>
     <row r="49" ht="28" customHeight="1" spans="1:15">
       <c r="A49" s="39"/>
-      <c r="B49" s="91"/>
-      <c r="C49" s="83"/>
-      <c r="D49" s="84"/>
+      <c r="B49" s="51"/>
+      <c r="C49" s="80"/>
+      <c r="D49" s="81"/>
       <c r="E49" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="F49" s="53"/>
-      <c r="G49" s="53"/>
-      <c r="H49" s="53"/>
-      <c r="I49" s="53"/>
-      <c r="J49" s="53"/>
-      <c r="K49" s="53"/>
-      <c r="L49" s="53"/>
-      <c r="M49" s="53"/>
-      <c r="N49" s="53"/>
-      <c r="O49" s="72"/>
-    </row>
-    <row r="50" spans="1:15">
+      <c r="F49" s="52"/>
+      <c r="G49" s="52"/>
+      <c r="H49" s="52"/>
+      <c r="I49" s="52"/>
+      <c r="J49" s="52"/>
+      <c r="K49" s="52"/>
+      <c r="L49" s="52"/>
+      <c r="M49" s="52"/>
+      <c r="N49" s="52"/>
+      <c r="O49" s="70"/>
+    </row>
+    <row r="50" ht="13.2" spans="1:15">
       <c r="A50" s="39"/>
-      <c r="B50" s="91"/>
-      <c r="C50" s="83" t="s">
+      <c r="B50" s="51"/>
+      <c r="C50" s="80" t="s">
         <v>73</v>
       </c>
-      <c r="D50" s="84" t="s">
+      <c r="D50" s="81" t="s">
         <v>74</v>
       </c>
       <c r="E50" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="F50" s="53"/>
-      <c r="G50" s="53"/>
-      <c r="H50" s="53"/>
-      <c r="I50" s="53"/>
-      <c r="J50" s="53"/>
-      <c r="K50" s="53"/>
-      <c r="L50" s="53"/>
-      <c r="M50" s="53"/>
-      <c r="N50" s="53"/>
-      <c r="O50" s="72"/>
+      <c r="F50" s="52"/>
+      <c r="G50" s="52"/>
+      <c r="H50" s="52"/>
+      <c r="I50" s="52"/>
+      <c r="J50" s="52"/>
+      <c r="K50" s="52"/>
+      <c r="L50" s="52"/>
+      <c r="M50" s="52"/>
+      <c r="N50" s="52"/>
+      <c r="O50" s="70"/>
     </row>
     <row r="51" ht="13.2" spans="1:15">
       <c r="A51" s="39"/>
-      <c r="B51" s="91"/>
-      <c r="C51" s="83"/>
-      <c r="D51" s="84"/>
+      <c r="B51" s="51"/>
+      <c r="C51" s="80"/>
+      <c r="D51" s="81"/>
       <c r="E51" s="43"/>
-      <c r="F51" s="53"/>
-      <c r="G51" s="53"/>
-      <c r="H51" s="53"/>
-      <c r="I51" s="53"/>
-      <c r="J51" s="53"/>
-      <c r="K51" s="53"/>
-      <c r="L51" s="53"/>
-      <c r="M51" s="53"/>
-      <c r="N51" s="53"/>
-      <c r="O51" s="72"/>
+      <c r="F51" s="52"/>
+      <c r="G51" s="52"/>
+      <c r="H51" s="52"/>
+      <c r="I51" s="52"/>
+      <c r="J51" s="52"/>
+      <c r="K51" s="52"/>
+      <c r="L51" s="52"/>
+      <c r="M51" s="52"/>
+      <c r="N51" s="52"/>
+      <c r="O51" s="70"/>
     </row>
     <row r="52" ht="13.2" spans="1:15">
       <c r="A52" s="39"/>
-      <c r="B52" s="91"/>
-      <c r="C52" s="83"/>
-      <c r="D52" s="84"/>
+      <c r="B52" s="51"/>
+      <c r="C52" s="80"/>
+      <c r="D52" s="81"/>
       <c r="E52" s="43"/>
-      <c r="F52" s="53"/>
-      <c r="G52" s="53"/>
-      <c r="H52" s="53"/>
-      <c r="I52" s="53"/>
-      <c r="J52" s="53"/>
-      <c r="K52" s="53"/>
-      <c r="L52" s="53"/>
-      <c r="M52" s="53"/>
-      <c r="N52" s="53"/>
-      <c r="O52" s="72"/>
+      <c r="F52" s="52"/>
+      <c r="G52" s="52"/>
+      <c r="H52" s="52"/>
+      <c r="I52" s="52"/>
+      <c r="J52" s="52"/>
+      <c r="K52" s="52"/>
+      <c r="L52" s="52"/>
+      <c r="M52" s="52"/>
+      <c r="N52" s="52"/>
+      <c r="O52" s="70"/>
     </row>
     <row r="53" ht="19" customHeight="1" spans="1:15">
-      <c r="A53" s="92"/>
-      <c r="B53" s="93"/>
-      <c r="C53" s="94"/>
-      <c r="D53" s="95"/>
-      <c r="E53" s="61"/>
-      <c r="F53" s="62"/>
-      <c r="G53" s="62"/>
-      <c r="H53" s="62"/>
-      <c r="I53" s="62"/>
-      <c r="J53" s="62"/>
-      <c r="K53" s="62"/>
-      <c r="L53" s="62"/>
-      <c r="M53" s="62"/>
-      <c r="N53" s="62"/>
-      <c r="O53" s="74"/>
+      <c r="A53" s="57"/>
+      <c r="B53" s="58"/>
+      <c r="C53" s="87"/>
+      <c r="D53" s="88"/>
+      <c r="E53" s="59"/>
+      <c r="F53" s="60"/>
+      <c r="G53" s="60"/>
+      <c r="H53" s="60"/>
+      <c r="I53" s="60"/>
+      <c r="J53" s="60"/>
+      <c r="K53" s="60"/>
+      <c r="L53" s="60"/>
+      <c r="M53" s="60"/>
+      <c r="N53" s="60"/>
+      <c r="O53" s="72"/>
     </row>
     <row r="54" ht="19" customHeight="1" spans="1:15">
-      <c r="A54" s="78" t="s">
+      <c r="A54" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="B54" s="90" t="s">
+      <c r="B54" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="C54" s="80" t="s">
+      <c r="C54" s="77" t="s">
         <v>78</v>
       </c>
-      <c r="D54" s="81" t="s">
+      <c r="D54" s="78" t="s">
         <v>74</v>
       </c>
-      <c r="E54" s="82" t="s">
+      <c r="E54" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="F54" s="82"/>
-      <c r="G54" s="82"/>
-      <c r="H54" s="82"/>
-      <c r="I54" s="82"/>
-      <c r="J54" s="82"/>
-      <c r="K54" s="82"/>
-      <c r="L54" s="82"/>
-      <c r="M54" s="82"/>
-      <c r="N54" s="82"/>
-      <c r="O54" s="100"/>
+      <c r="F54" s="79"/>
+      <c r="G54" s="79"/>
+      <c r="H54" s="79"/>
+      <c r="I54" s="79"/>
+      <c r="J54" s="79"/>
+      <c r="K54" s="79"/>
+      <c r="L54" s="79"/>
+      <c r="M54" s="79"/>
+      <c r="N54" s="79"/>
+      <c r="O54" s="92"/>
     </row>
     <row r="55" ht="13.2" spans="1:15">
       <c r="A55" s="39"/>
-      <c r="B55" s="91"/>
-      <c r="C55" s="83"/>
-      <c r="D55" s="84"/>
+      <c r="B55" s="51"/>
+      <c r="C55" s="80"/>
+      <c r="D55" s="81"/>
       <c r="E55" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="F55" s="53"/>
-      <c r="G55" s="53"/>
-      <c r="H55" s="53"/>
-      <c r="I55" s="53"/>
-      <c r="J55" s="53"/>
-      <c r="K55" s="53"/>
-      <c r="L55" s="53"/>
-      <c r="M55" s="53"/>
-      <c r="N55" s="53"/>
-      <c r="O55" s="72"/>
+      <c r="F55" s="52"/>
+      <c r="G55" s="52"/>
+      <c r="H55" s="52"/>
+      <c r="I55" s="52"/>
+      <c r="J55" s="52"/>
+      <c r="K55" s="52"/>
+      <c r="L55" s="52"/>
+      <c r="M55" s="52"/>
+      <c r="N55" s="52"/>
+      <c r="O55" s="70"/>
     </row>
     <row r="56" ht="13.2" spans="1:15">
       <c r="A56" s="39"/>
-      <c r="B56" s="91"/>
-      <c r="C56" s="83"/>
-      <c r="D56" s="84"/>
+      <c r="B56" s="51"/>
+      <c r="C56" s="80"/>
+      <c r="D56" s="81"/>
       <c r="E56" s="43"/>
-      <c r="F56" s="53"/>
-      <c r="G56" s="53"/>
-      <c r="H56" s="53"/>
-      <c r="I56" s="53"/>
-      <c r="J56" s="53"/>
-      <c r="K56" s="53"/>
-      <c r="L56" s="53"/>
-      <c r="M56" s="53"/>
-      <c r="N56" s="53"/>
-      <c r="O56" s="72"/>
+      <c r="F56" s="52"/>
+      <c r="G56" s="52"/>
+      <c r="H56" s="52"/>
+      <c r="I56" s="52"/>
+      <c r="J56" s="52"/>
+      <c r="K56" s="52"/>
+      <c r="L56" s="52"/>
+      <c r="M56" s="52"/>
+      <c r="N56" s="52"/>
+      <c r="O56" s="70"/>
     </row>
     <row r="57" ht="13.2" spans="1:15">
       <c r="A57" s="39"/>
-      <c r="B57" s="91"/>
-      <c r="C57" s="83"/>
-      <c r="D57" s="84"/>
+      <c r="B57" s="51"/>
+      <c r="C57" s="80"/>
+      <c r="D57" s="81"/>
       <c r="E57" s="43"/>
-      <c r="F57" s="53"/>
-      <c r="G57" s="53"/>
-      <c r="H57" s="53"/>
-      <c r="I57" s="53"/>
-      <c r="J57" s="53"/>
-      <c r="K57" s="53"/>
-      <c r="L57" s="53"/>
-      <c r="M57" s="53"/>
-      <c r="N57" s="53"/>
-      <c r="O57" s="72"/>
+      <c r="F57" s="52"/>
+      <c r="G57" s="52"/>
+      <c r="H57" s="52"/>
+      <c r="I57" s="52"/>
+      <c r="J57" s="52"/>
+      <c r="K57" s="52"/>
+      <c r="L57" s="52"/>
+      <c r="M57" s="52"/>
+      <c r="N57" s="52"/>
+      <c r="O57" s="70"/>
     </row>
     <row r="58" ht="13.8" spans="1:15">
       <c r="A58" s="39"/>
-      <c r="B58" s="91"/>
-      <c r="C58" s="83" t="s">
+      <c r="B58" s="51"/>
+      <c r="C58" s="80" t="s">
         <v>80</v>
       </c>
-      <c r="D58" s="84" t="s">
+      <c r="D58" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="E58" s="97" t="s">
+      <c r="E58" s="89" t="s">
         <v>81</v>
       </c>
-      <c r="F58" s="53"/>
-      <c r="G58" s="53"/>
-      <c r="H58" s="53"/>
-      <c r="I58" s="53"/>
-      <c r="J58" s="53"/>
-      <c r="K58" s="53"/>
-      <c r="L58" s="53"/>
-      <c r="M58" s="53"/>
-      <c r="N58" s="53"/>
-      <c r="O58" s="72"/>
+      <c r="F58" s="52"/>
+      <c r="G58" s="52"/>
+      <c r="H58" s="52"/>
+      <c r="I58" s="52"/>
+      <c r="J58" s="52"/>
+      <c r="K58" s="52"/>
+      <c r="L58" s="52"/>
+      <c r="M58" s="52"/>
+      <c r="N58" s="52"/>
+      <c r="O58" s="70"/>
     </row>
     <row r="59" ht="13.8" spans="1:15">
       <c r="A59" s="39"/>
-      <c r="B59" s="91"/>
-      <c r="C59" s="83"/>
-      <c r="D59" s="84"/>
-      <c r="E59" s="97" t="s">
+      <c r="B59" s="51"/>
+      <c r="C59" s="80"/>
+      <c r="D59" s="81"/>
+      <c r="E59" s="89" t="s">
         <v>82</v>
       </c>
-      <c r="F59" s="53"/>
-      <c r="G59" s="53"/>
-      <c r="H59" s="53"/>
-      <c r="I59" s="53"/>
-      <c r="J59" s="53"/>
-      <c r="K59" s="53"/>
-      <c r="L59" s="53"/>
-      <c r="M59" s="53"/>
-      <c r="N59" s="53"/>
-      <c r="O59" s="72"/>
+      <c r="F59" s="52"/>
+      <c r="G59" s="52"/>
+      <c r="H59" s="52"/>
+      <c r="I59" s="52"/>
+      <c r="J59" s="52"/>
+      <c r="K59" s="52"/>
+      <c r="L59" s="52"/>
+      <c r="M59" s="52"/>
+      <c r="N59" s="52"/>
+      <c r="O59" s="70"/>
     </row>
     <row r="60" ht="14.55" spans="1:15">
       <c r="A60" s="44"/>
-      <c r="B60" s="96"/>
-      <c r="C60" s="88"/>
-      <c r="D60" s="89"/>
-      <c r="E60" s="98" t="s">
+      <c r="B60" s="53"/>
+      <c r="C60" s="85"/>
+      <c r="D60" s="86"/>
+      <c r="E60" s="90" t="s">
         <v>83</v>
       </c>
-      <c r="F60" s="56"/>
-      <c r="G60" s="56"/>
-      <c r="H60" s="56"/>
-      <c r="I60" s="56"/>
-      <c r="J60" s="56"/>
-      <c r="K60" s="56"/>
-      <c r="L60" s="56"/>
-      <c r="M60" s="56"/>
-      <c r="N60" s="56"/>
-      <c r="O60" s="73"/>
+      <c r="F60" s="54"/>
+      <c r="G60" s="54"/>
+      <c r="H60" s="54"/>
+      <c r="I60" s="54"/>
+      <c r="J60" s="54"/>
+      <c r="K60" s="54"/>
+      <c r="L60" s="54"/>
+      <c r="M60" s="54"/>
+      <c r="N60" s="54"/>
+      <c r="O60" s="71"/>
     </row>
     <row r="61" ht="13.8" spans="1:15">
-      <c r="A61" s="78" t="s">
+      <c r="A61" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="B61" s="90" t="s">
+      <c r="B61" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="C61" s="80" t="s">
+      <c r="C61" s="77" t="s">
         <v>85</v>
       </c>
-      <c r="D61" s="81" t="s">
+      <c r="D61" s="78" t="s">
         <v>86</v>
       </c>
-      <c r="E61" s="82" t="s">
+      <c r="E61" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="F61" s="82"/>
-      <c r="G61" s="82"/>
-      <c r="H61" s="82"/>
-      <c r="I61" s="82"/>
-      <c r="J61" s="82"/>
-      <c r="K61" s="82"/>
-      <c r="L61" s="82"/>
-      <c r="M61" s="82"/>
-      <c r="N61" s="82"/>
-      <c r="O61" s="100"/>
+      <c r="F61" s="79"/>
+      <c r="G61" s="79"/>
+      <c r="H61" s="79"/>
+      <c r="I61" s="79"/>
+      <c r="J61" s="79"/>
+      <c r="K61" s="79"/>
+      <c r="L61" s="79"/>
+      <c r="M61" s="79"/>
+      <c r="N61" s="79"/>
+      <c r="O61" s="92"/>
     </row>
     <row r="62" ht="13.8" spans="1:15">
       <c r="A62" s="39"/>
-      <c r="B62" s="91"/>
-      <c r="C62" s="83"/>
-      <c r="D62" s="84"/>
-      <c r="E62" s="97" t="s">
+      <c r="B62" s="51"/>
+      <c r="C62" s="80"/>
+      <c r="D62" s="81"/>
+      <c r="E62" s="89" t="s">
         <v>87</v>
       </c>
-      <c r="F62" s="53"/>
-      <c r="G62" s="53"/>
-      <c r="H62" s="53"/>
-      <c r="I62" s="53"/>
-      <c r="J62" s="53"/>
-      <c r="K62" s="53"/>
-      <c r="L62" s="53"/>
-      <c r="M62" s="53"/>
-      <c r="N62" s="53"/>
-      <c r="O62" s="72"/>
+      <c r="F62" s="52"/>
+      <c r="G62" s="52"/>
+      <c r="H62" s="52"/>
+      <c r="I62" s="52"/>
+      <c r="J62" s="52"/>
+      <c r="K62" s="52"/>
+      <c r="L62" s="52"/>
+      <c r="M62" s="52"/>
+      <c r="N62" s="52"/>
+      <c r="O62" s="70"/>
     </row>
     <row r="63" ht="13.8" spans="1:15">
       <c r="A63" s="39"/>
-      <c r="B63" s="91"/>
-      <c r="C63" s="83"/>
-      <c r="D63" s="84"/>
-      <c r="E63" s="97" t="s">
+      <c r="B63" s="51"/>
+      <c r="C63" s="80"/>
+      <c r="D63" s="81"/>
+      <c r="E63" s="89" t="s">
         <v>88</v>
       </c>
-      <c r="F63" s="53"/>
-      <c r="G63" s="53"/>
-      <c r="H63" s="53"/>
-      <c r="I63" s="53"/>
-      <c r="J63" s="53"/>
-      <c r="K63" s="53"/>
-      <c r="L63" s="53"/>
-      <c r="M63" s="53"/>
-      <c r="N63" s="53"/>
-      <c r="O63" s="72"/>
+      <c r="F63" s="52"/>
+      <c r="G63" s="52"/>
+      <c r="H63" s="52"/>
+      <c r="I63" s="52"/>
+      <c r="J63" s="52"/>
+      <c r="K63" s="52"/>
+      <c r="L63" s="52"/>
+      <c r="M63" s="52"/>
+      <c r="N63" s="52"/>
+      <c r="O63" s="70"/>
     </row>
     <row r="64" ht="13.8" spans="1:15">
       <c r="A64" s="39"/>
-      <c r="B64" s="91"/>
-      <c r="C64" s="83"/>
-      <c r="D64" s="84"/>
-      <c r="E64" s="86" t="s">
+      <c r="B64" s="51"/>
+      <c r="C64" s="80"/>
+      <c r="D64" s="81"/>
+      <c r="E64" s="83" t="s">
         <v>31</v>
       </c>
-      <c r="F64" s="86"/>
-      <c r="G64" s="86"/>
-      <c r="H64" s="86"/>
-      <c r="I64" s="86"/>
-      <c r="J64" s="86"/>
-      <c r="K64" s="86"/>
-      <c r="L64" s="86"/>
-      <c r="M64" s="86"/>
-      <c r="N64" s="86"/>
-      <c r="O64" s="101"/>
+      <c r="F64" s="83"/>
+      <c r="G64" s="83"/>
+      <c r="H64" s="83"/>
+      <c r="I64" s="83"/>
+      <c r="J64" s="83"/>
+      <c r="K64" s="83"/>
+      <c r="L64" s="83"/>
+      <c r="M64" s="83"/>
+      <c r="N64" s="83"/>
+      <c r="O64" s="93"/>
     </row>
     <row r="65" ht="13.8" spans="1:15">
       <c r="A65" s="39"/>
-      <c r="B65" s="91"/>
-      <c r="C65" s="83"/>
-      <c r="D65" s="84"/>
-      <c r="E65" s="97" t="s">
+      <c r="B65" s="51"/>
+      <c r="C65" s="80"/>
+      <c r="D65" s="81"/>
+      <c r="E65" s="89" t="s">
         <v>89</v>
       </c>
-      <c r="F65" s="53"/>
-      <c r="G65" s="53"/>
-      <c r="H65" s="53"/>
-      <c r="I65" s="53"/>
-      <c r="J65" s="53"/>
-      <c r="K65" s="53"/>
-      <c r="L65" s="53"/>
-      <c r="M65" s="53"/>
-      <c r="N65" s="53"/>
-      <c r="O65" s="72"/>
+      <c r="F65" s="52"/>
+      <c r="G65" s="52"/>
+      <c r="H65" s="52"/>
+      <c r="I65" s="52"/>
+      <c r="J65" s="52"/>
+      <c r="K65" s="52"/>
+      <c r="L65" s="52"/>
+      <c r="M65" s="52"/>
+      <c r="N65" s="52"/>
+      <c r="O65" s="70"/>
     </row>
     <row r="66" ht="27.6" spans="1:15">
       <c r="A66" s="39"/>
-      <c r="B66" s="91"/>
-      <c r="C66" s="83"/>
-      <c r="D66" s="84"/>
-      <c r="E66" s="97" t="s">
+      <c r="B66" s="51"/>
+      <c r="C66" s="80"/>
+      <c r="D66" s="81"/>
+      <c r="E66" s="89" t="s">
         <v>90</v>
       </c>
-      <c r="F66" s="53"/>
-      <c r="G66" s="53"/>
-      <c r="H66" s="53"/>
-      <c r="I66" s="53"/>
-      <c r="J66" s="53"/>
-      <c r="K66" s="53"/>
-      <c r="L66" s="53"/>
-      <c r="M66" s="53"/>
-      <c r="N66" s="53"/>
-      <c r="O66" s="72"/>
+      <c r="F66" s="52"/>
+      <c r="G66" s="52"/>
+      <c r="H66" s="52"/>
+      <c r="I66" s="52"/>
+      <c r="J66" s="52"/>
+      <c r="K66" s="52"/>
+      <c r="L66" s="52"/>
+      <c r="M66" s="52"/>
+      <c r="N66" s="52"/>
+      <c r="O66" s="70"/>
     </row>
     <row r="67" ht="13.8" spans="1:15">
       <c r="A67" s="39"/>
-      <c r="B67" s="91"/>
-      <c r="C67" s="83"/>
-      <c r="D67" s="84"/>
-      <c r="E67" s="97" t="s">
+      <c r="B67" s="51"/>
+      <c r="C67" s="80"/>
+      <c r="D67" s="81"/>
+      <c r="E67" s="89" t="s">
         <v>91</v>
       </c>
-      <c r="F67" s="53"/>
-      <c r="G67" s="53"/>
-      <c r="H67" s="53"/>
-      <c r="I67" s="53"/>
-      <c r="J67" s="53"/>
-      <c r="K67" s="53"/>
-      <c r="L67" s="53"/>
-      <c r="M67" s="53"/>
-      <c r="N67" s="53"/>
-      <c r="O67" s="72"/>
+      <c r="F67" s="52"/>
+      <c r="G67" s="52"/>
+      <c r="H67" s="52"/>
+      <c r="I67" s="52"/>
+      <c r="J67" s="52"/>
+      <c r="K67" s="52"/>
+      <c r="L67" s="52"/>
+      <c r="M67" s="52"/>
+      <c r="N67" s="52"/>
+      <c r="O67" s="70"/>
     </row>
     <row r="68" ht="14.55" spans="1:15">
       <c r="A68" s="44"/>
-      <c r="B68" s="96"/>
-      <c r="C68" s="88"/>
-      <c r="D68" s="89"/>
-      <c r="E68" s="98" t="s">
+      <c r="B68" s="53"/>
+      <c r="C68" s="85"/>
+      <c r="D68" s="86"/>
+      <c r="E68" s="90" t="s">
         <v>92</v>
       </c>
-      <c r="F68" s="56"/>
-      <c r="G68" s="56"/>
-      <c r="H68" s="56"/>
-      <c r="I68" s="56"/>
-      <c r="J68" s="56"/>
-      <c r="K68" s="56"/>
-      <c r="L68" s="56"/>
-      <c r="M68" s="56"/>
-      <c r="N68" s="56"/>
-      <c r="O68" s="73"/>
+      <c r="F68" s="54"/>
+      <c r="G68" s="54"/>
+      <c r="H68" s="54"/>
+      <c r="I68" s="54"/>
+      <c r="J68" s="54"/>
+      <c r="K68" s="54"/>
+      <c r="L68" s="54"/>
+      <c r="M68" s="54"/>
+      <c r="N68" s="54"/>
+      <c r="O68" s="71"/>
     </row>
     <row r="69" ht="13.8" spans="1:15">
       <c r="A69" s="47" t="s">
@@ -3955,86 +3902,86 @@
       <c r="B69" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="C69" s="103" t="s">
+      <c r="C69" s="77" t="s">
         <v>94</v>
       </c>
-      <c r="D69" s="104" t="s">
+      <c r="D69" s="78" t="s">
         <v>95</v>
       </c>
-      <c r="E69" s="105" t="s">
+      <c r="E69" s="95" t="s">
         <v>96</v>
       </c>
-      <c r="F69" s="106"/>
-      <c r="G69" s="106"/>
-      <c r="H69" s="106"/>
-      <c r="I69" s="106"/>
-      <c r="J69" s="106"/>
-      <c r="K69" s="106"/>
-      <c r="L69" s="106"/>
-      <c r="M69" s="106"/>
-      <c r="N69" s="106"/>
-      <c r="O69" s="116"/>
+      <c r="F69" s="50"/>
+      <c r="G69" s="50"/>
+      <c r="H69" s="50"/>
+      <c r="I69" s="50"/>
+      <c r="J69" s="50"/>
+      <c r="K69" s="50"/>
+      <c r="L69" s="50"/>
+      <c r="M69" s="50"/>
+      <c r="N69" s="50"/>
+      <c r="O69" s="69"/>
     </row>
     <row r="70" ht="27.6" spans="1:15">
-      <c r="A70" s="51"/>
-      <c r="B70" s="52"/>
-      <c r="C70" s="107"/>
-      <c r="D70" s="108"/>
-      <c r="E70" s="97" t="s">
+      <c r="A70" s="39"/>
+      <c r="B70" s="51"/>
+      <c r="C70" s="80"/>
+      <c r="D70" s="81"/>
+      <c r="E70" s="89" t="s">
         <v>97</v>
       </c>
-      <c r="F70" s="109"/>
-      <c r="G70" s="109"/>
-      <c r="H70" s="109"/>
-      <c r="I70" s="109"/>
-      <c r="J70" s="109"/>
-      <c r="K70" s="109"/>
-      <c r="L70" s="109"/>
-      <c r="M70" s="109"/>
-      <c r="N70" s="109"/>
-      <c r="O70" s="117"/>
+      <c r="F70" s="52"/>
+      <c r="G70" s="52"/>
+      <c r="H70" s="52"/>
+      <c r="I70" s="52"/>
+      <c r="J70" s="52"/>
+      <c r="K70" s="52"/>
+      <c r="L70" s="52"/>
+      <c r="M70" s="52"/>
+      <c r="N70" s="52"/>
+      <c r="O70" s="70"/>
     </row>
     <row r="71" ht="27" customHeight="1" spans="1:15">
-      <c r="A71" s="51"/>
-      <c r="B71" s="52"/>
-      <c r="C71" s="107"/>
-      <c r="D71" s="84" t="s">
+      <c r="A71" s="39"/>
+      <c r="B71" s="51"/>
+      <c r="C71" s="80"/>
+      <c r="D71" s="81" t="s">
         <v>60</v>
       </c>
-      <c r="E71" s="97" t="s">
+      <c r="E71" s="89" t="s">
         <v>98</v>
       </c>
-      <c r="F71" s="109"/>
-      <c r="G71" s="109"/>
-      <c r="H71" s="109"/>
-      <c r="I71" s="109"/>
-      <c r="J71" s="109"/>
-      <c r="K71" s="109"/>
-      <c r="L71" s="109"/>
-      <c r="M71" s="109"/>
-      <c r="N71" s="109"/>
-      <c r="O71" s="117"/>
+      <c r="F71" s="52"/>
+      <c r="G71" s="52"/>
+      <c r="H71" s="52"/>
+      <c r="I71" s="52"/>
+      <c r="J71" s="52"/>
+      <c r="K71" s="52"/>
+      <c r="L71" s="52"/>
+      <c r="M71" s="52"/>
+      <c r="N71" s="52"/>
+      <c r="O71" s="70"/>
     </row>
     <row r="72" ht="42.15" spans="1:15">
-      <c r="A72" s="54"/>
-      <c r="B72" s="55"/>
-      <c r="C72" s="110"/>
-      <c r="D72" s="89" t="s">
+      <c r="A72" s="44"/>
+      <c r="B72" s="53"/>
+      <c r="C72" s="85"/>
+      <c r="D72" s="86" t="s">
         <v>99</v>
       </c>
-      <c r="E72" s="98" t="s">
+      <c r="E72" s="90" t="s">
         <v>100</v>
       </c>
-      <c r="F72" s="111"/>
-      <c r="G72" s="111"/>
-      <c r="H72" s="111"/>
-      <c r="I72" s="111"/>
-      <c r="J72" s="111"/>
-      <c r="K72" s="111"/>
-      <c r="L72" s="111"/>
-      <c r="M72" s="111"/>
-      <c r="N72" s="111"/>
-      <c r="O72" s="118"/>
+      <c r="F72" s="54"/>
+      <c r="G72" s="54"/>
+      <c r="H72" s="54"/>
+      <c r="I72" s="54"/>
+      <c r="J72" s="54"/>
+      <c r="K72" s="54"/>
+      <c r="L72" s="54"/>
+      <c r="M72" s="54"/>
+      <c r="N72" s="54"/>
+      <c r="O72" s="71"/>
     </row>
     <row r="73" ht="13.8" spans="1:15">
       <c r="A73" s="47" t="s">
@@ -4043,121 +3990,121 @@
       <c r="B73" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="C73" s="103" t="s">
+      <c r="C73" s="77" t="s">
         <v>102</v>
       </c>
-      <c r="D73" s="104" t="s">
+      <c r="D73" s="78" t="s">
         <v>95</v>
       </c>
-      <c r="E73" s="105" t="s">
+      <c r="E73" s="95" t="s">
         <v>103</v>
       </c>
-      <c r="F73" s="106"/>
-      <c r="G73" s="106"/>
-      <c r="H73" s="106"/>
-      <c r="I73" s="106"/>
-      <c r="J73" s="106"/>
-      <c r="K73" s="106"/>
-      <c r="L73" s="106"/>
-      <c r="M73" s="106"/>
-      <c r="N73" s="106"/>
-      <c r="O73" s="116"/>
+      <c r="F73" s="50"/>
+      <c r="G73" s="50"/>
+      <c r="H73" s="50"/>
+      <c r="I73" s="50"/>
+      <c r="J73" s="50"/>
+      <c r="K73" s="50"/>
+      <c r="L73" s="50"/>
+      <c r="M73" s="50"/>
+      <c r="N73" s="50"/>
+      <c r="O73" s="69"/>
     </row>
     <row r="74" ht="28" customHeight="1" spans="1:15">
-      <c r="A74" s="59"/>
-      <c r="B74" s="60"/>
-      <c r="C74" s="112"/>
-      <c r="D74" s="113"/>
-      <c r="E74" s="114" t="s">
+      <c r="A74" s="57"/>
+      <c r="B74" s="58"/>
+      <c r="C74" s="87"/>
+      <c r="D74" s="88"/>
+      <c r="E74" s="96" t="s">
         <v>104</v>
       </c>
-      <c r="F74" s="115"/>
-      <c r="G74" s="115"/>
-      <c r="H74" s="115"/>
-      <c r="I74" s="115"/>
-      <c r="J74" s="115"/>
-      <c r="K74" s="115"/>
-      <c r="L74" s="115"/>
-      <c r="M74" s="115"/>
-      <c r="N74" s="115"/>
-      <c r="O74" s="119"/>
-    </row>
-    <row r="75" spans="3:5">
+      <c r="F74" s="60"/>
+      <c r="G74" s="60"/>
+      <c r="H74" s="60"/>
+      <c r="I74" s="60"/>
+      <c r="J74" s="60"/>
+      <c r="K74" s="60"/>
+      <c r="L74" s="60"/>
+      <c r="M74" s="60"/>
+      <c r="N74" s="60"/>
+      <c r="O74" s="72"/>
+    </row>
+    <row r="75" ht="13.2" spans="3:5">
       <c r="C75" s="7"/>
       <c r="D75" s="7"/>
       <c r="E75" s="7"/>
     </row>
-    <row r="76" spans="3:5">
+    <row r="76" ht="13.2" spans="3:5">
       <c r="C76" s="7"/>
       <c r="D76" s="7"/>
       <c r="E76" s="7"/>
     </row>
-    <row r="77" spans="3:5">
+    <row r="77" ht="13.2" spans="3:5">
       <c r="C77" s="7"/>
       <c r="D77" s="7"/>
       <c r="E77" s="7"/>
     </row>
-    <row r="78" spans="3:5">
+    <row r="78" ht="13.2" spans="3:5">
       <c r="C78" s="7"/>
       <c r="D78" s="7"/>
       <c r="E78" s="7"/>
     </row>
-    <row r="79" spans="3:5">
+    <row r="79" ht="13.2" spans="3:5">
       <c r="C79" s="7"/>
       <c r="D79" s="7"/>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="3:5">
+    <row r="80" ht="13.2" spans="3:5">
       <c r="C80" s="7"/>
       <c r="D80" s="7"/>
       <c r="E80" s="7"/>
     </row>
-    <row r="81" spans="3:5">
+    <row r="81" ht="13.2" spans="3:5">
       <c r="C81" s="7"/>
       <c r="D81" s="7"/>
       <c r="E81" s="7"/>
     </row>
-    <row r="82" spans="3:5">
+    <row r="82" ht="13.2" spans="3:5">
       <c r="C82" s="7"/>
       <c r="D82" s="7"/>
       <c r="E82" s="7"/>
     </row>
-    <row r="83" spans="3:5">
+    <row r="83" ht="13.2" spans="3:5">
       <c r="C83" s="7"/>
       <c r="D83" s="7"/>
       <c r="E83" s="7"/>
     </row>
-    <row r="84" spans="3:5">
+    <row r="84" ht="13.2" spans="3:5">
       <c r="C84" s="7"/>
       <c r="D84" s="7"/>
       <c r="E84" s="7"/>
     </row>
-    <row r="85" spans="3:5">
+    <row r="85" ht="13.2" spans="3:5">
       <c r="C85" s="7"/>
       <c r="D85" s="7"/>
       <c r="E85" s="7"/>
     </row>
-    <row r="86" spans="3:5">
+    <row r="86" ht="13.2" spans="3:5">
       <c r="C86" s="7"/>
       <c r="D86" s="7"/>
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="3:5">
+    <row r="87" ht="13.2" spans="3:5">
       <c r="C87" s="7"/>
       <c r="D87" s="7"/>
       <c r="E87" s="7"/>
     </row>
-    <row r="88" spans="3:5">
+    <row r="88" ht="13.2" spans="3:5">
       <c r="C88" s="7"/>
       <c r="D88" s="7"/>
       <c r="E88" s="7"/>
     </row>
-    <row r="89" spans="3:5">
+    <row r="89" ht="13.2" spans="3:5">
       <c r="C89" s="7"/>
       <c r="D89" s="7"/>
       <c r="E89" s="7"/>
     </row>
-    <row r="90" spans="3:5">
+    <row r="90" ht="13.2" spans="3:5">
       <c r="C90" s="7"/>
       <c r="D90" s="7"/>
       <c r="E90" s="7"/>
@@ -8621,8 +8568,8 @@
   <sheetPr/>
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21:B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="13.2"/>
@@ -8633,7 +8580,7 @@
     <col min="4" max="4" width="42.4444444444444" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="50.4" spans="1:13">
+    <row r="1" ht="16.8" spans="1:13">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -8650,7 +8597,7 @@
       <c r="J1" s="20"/>
       <c r="K1" s="20"/>
       <c r="L1" s="20"/>
-      <c r="M1" s="63"/>
+      <c r="M1" s="61"/>
     </row>
     <row r="2" ht="16.8" spans="1:13">
       <c r="A2" s="21" t="s">
@@ -8669,7 +8616,7 @@
       <c r="J2" s="25"/>
       <c r="K2" s="25"/>
       <c r="L2" s="25"/>
-      <c r="M2" s="64"/>
+      <c r="M2" s="62"/>
     </row>
     <row r="3" ht="16.8" spans="1:13">
       <c r="A3" s="21" t="s">
@@ -8688,7 +8635,7 @@
       <c r="J3" s="25"/>
       <c r="K3" s="25"/>
       <c r="L3" s="25"/>
-      <c r="M3" s="64"/>
+      <c r="M3" s="62"/>
     </row>
     <row r="4" ht="16.8" spans="1:13">
       <c r="A4" s="21" t="s">
@@ -8707,7 +8654,7 @@
       <c r="J4" s="28"/>
       <c r="K4" s="28"/>
       <c r="L4" s="28"/>
-      <c r="M4" s="65"/>
+      <c r="M4" s="63"/>
     </row>
     <row r="5" ht="28.35" spans="1:13">
       <c r="A5" s="29" t="s">
@@ -8734,9 +8681,9 @@
       <c r="L5" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="66"/>
-    </row>
-    <row r="6" ht="42.15" spans="1:13">
+      <c r="M5" s="64"/>
+    </row>
+    <row r="6" ht="14.55" spans="1:13">
       <c r="A6" s="32" t="s">
         <v>13</v>
       </c>
@@ -8773,7 +8720,7 @@
       <c r="L6" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="M6" s="67" t="s">
+      <c r="M6" s="65" t="s">
         <v>19</v>
       </c>
     </row>
@@ -8798,7 +8745,7 @@
       <c r="J7" s="38"/>
       <c r="K7" s="38"/>
       <c r="L7" s="38"/>
-      <c r="M7" s="68"/>
+      <c r="M7" s="66"/>
     </row>
     <row r="8" ht="27.6" spans="1:13">
       <c r="A8" s="39"/>
@@ -8817,7 +8764,7 @@
       <c r="J8" s="42"/>
       <c r="K8" s="42"/>
       <c r="L8" s="42"/>
-      <c r="M8" s="69"/>
+      <c r="M8" s="67"/>
     </row>
     <row r="9" ht="76" customHeight="1" spans="1:13">
       <c r="A9" s="39"/>
@@ -8834,9 +8781,9 @@
       <c r="J9" s="42"/>
       <c r="K9" s="42"/>
       <c r="L9" s="42"/>
-      <c r="M9" s="69"/>
-    </row>
-    <row r="10" ht="55.2" spans="1:13">
+      <c r="M9" s="67"/>
+    </row>
+    <row r="10" ht="41.4" spans="1:13">
       <c r="A10" s="39"/>
       <c r="B10" s="35"/>
       <c r="C10" s="43" t="s">
@@ -8851,9 +8798,9 @@
       <c r="J10" s="42"/>
       <c r="K10" s="42"/>
       <c r="L10" s="42"/>
-      <c r="M10" s="69"/>
-    </row>
-    <row r="11" ht="55.2" spans="1:13">
+      <c r="M10" s="67"/>
+    </row>
+    <row r="11" ht="41.4" spans="1:13">
       <c r="A11" s="39"/>
       <c r="B11" s="35"/>
       <c r="C11" s="43" t="s">
@@ -8868,9 +8815,9 @@
       <c r="J11" s="42"/>
       <c r="K11" s="42"/>
       <c r="L11" s="42"/>
-      <c r="M11" s="69"/>
-    </row>
-    <row r="12" ht="55.2" spans="1:13">
+      <c r="M11" s="67"/>
+    </row>
+    <row r="12" ht="27.6" spans="1:13">
       <c r="A12" s="39"/>
       <c r="B12" s="35"/>
       <c r="C12" s="43" t="s">
@@ -8885,7 +8832,7 @@
       <c r="J12" s="42"/>
       <c r="K12" s="42"/>
       <c r="L12" s="42"/>
-      <c r="M12" s="69"/>
+      <c r="M12" s="67"/>
     </row>
     <row r="13" ht="28.35" spans="1:13">
       <c r="A13" s="44"/>
@@ -8902,7 +8849,7 @@
       <c r="J13" s="46"/>
       <c r="K13" s="46"/>
       <c r="L13" s="46"/>
-      <c r="M13" s="70"/>
+      <c r="M13" s="68"/>
     </row>
     <row r="14" ht="27.6" spans="1:13">
       <c r="A14" s="47" t="s">
@@ -8923,109 +8870,109 @@
       <c r="J14" s="50"/>
       <c r="K14" s="50"/>
       <c r="L14" s="50"/>
-      <c r="M14" s="71"/>
+      <c r="M14" s="69"/>
     </row>
     <row r="15" ht="27.6" spans="1:13">
-      <c r="A15" s="51"/>
-      <c r="B15" s="52"/>
+      <c r="A15" s="39"/>
+      <c r="B15" s="51"/>
       <c r="C15" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="D15" s="53"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="53"/>
-      <c r="H15" s="53"/>
-      <c r="I15" s="53"/>
-      <c r="J15" s="53"/>
-      <c r="K15" s="53"/>
-      <c r="L15" s="53"/>
-      <c r="M15" s="72"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="52"/>
+      <c r="L15" s="52"/>
+      <c r="M15" s="70"/>
     </row>
     <row r="16" ht="27.6" spans="1:13">
-      <c r="A16" s="51"/>
-      <c r="B16" s="52"/>
+      <c r="A16" s="39"/>
+      <c r="B16" s="51"/>
       <c r="C16" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="D16" s="53"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="53"/>
-      <c r="G16" s="53"/>
-      <c r="H16" s="53"/>
-      <c r="I16" s="53"/>
-      <c r="J16" s="53"/>
-      <c r="K16" s="53"/>
-      <c r="L16" s="53"/>
-      <c r="M16" s="72"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="52"/>
+      <c r="L16" s="52"/>
+      <c r="M16" s="70"/>
     </row>
     <row r="17" ht="27.6" spans="1:13">
-      <c r="A17" s="51"/>
-      <c r="B17" s="52"/>
+      <c r="A17" s="39"/>
+      <c r="B17" s="51"/>
       <c r="C17" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="53"/>
-      <c r="H17" s="53"/>
-      <c r="I17" s="53"/>
-      <c r="J17" s="53"/>
-      <c r="K17" s="53"/>
-      <c r="L17" s="53"/>
-      <c r="M17" s="72"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="52"/>
+      <c r="L17" s="52"/>
+      <c r="M17" s="70"/>
     </row>
     <row r="18" ht="41.4" spans="1:13">
-      <c r="A18" s="51"/>
-      <c r="B18" s="52"/>
+      <c r="A18" s="39"/>
+      <c r="B18" s="51"/>
       <c r="C18" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="D18" s="53"/>
-      <c r="E18" s="53"/>
-      <c r="F18" s="53"/>
-      <c r="G18" s="53"/>
-      <c r="H18" s="53"/>
-      <c r="I18" s="53"/>
-      <c r="J18" s="53"/>
-      <c r="K18" s="53"/>
-      <c r="L18" s="53"/>
-      <c r="M18" s="72"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="52"/>
+      <c r="J18" s="52"/>
+      <c r="K18" s="52"/>
+      <c r="L18" s="52"/>
+      <c r="M18" s="70"/>
     </row>
     <row r="19" ht="41.4" spans="1:13">
-      <c r="A19" s="51"/>
-      <c r="B19" s="52"/>
+      <c r="A19" s="39"/>
+      <c r="B19" s="51"/>
       <c r="C19" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="D19" s="53"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="53"/>
-      <c r="G19" s="53"/>
-      <c r="H19" s="53"/>
-      <c r="I19" s="53"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="53"/>
-      <c r="L19" s="53"/>
-      <c r="M19" s="72"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="52"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="52"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="52"/>
+      <c r="K19" s="52"/>
+      <c r="L19" s="52"/>
+      <c r="M19" s="70"/>
     </row>
     <row r="20" ht="28.35" spans="1:13">
-      <c r="A20" s="54"/>
-      <c r="B20" s="55"/>
+      <c r="A20" s="44"/>
+      <c r="B20" s="53"/>
       <c r="C20" s="45" t="s">
         <v>120</v>
       </c>
-      <c r="D20" s="56"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="56"/>
-      <c r="H20" s="56"/>
-      <c r="I20" s="56"/>
-      <c r="J20" s="56"/>
-      <c r="K20" s="56"/>
-      <c r="L20" s="56"/>
-      <c r="M20" s="73"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="54"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="54"/>
+      <c r="H20" s="54"/>
+      <c r="I20" s="54"/>
+      <c r="J20" s="54"/>
+      <c r="K20" s="54"/>
+      <c r="L20" s="54"/>
+      <c r="M20" s="71"/>
     </row>
     <row r="21" ht="27.6" spans="1:13">
       <c r="A21" s="47" t="s">
@@ -9046,245 +8993,245 @@
       <c r="J21" s="50"/>
       <c r="K21" s="50"/>
       <c r="L21" s="50"/>
-      <c r="M21" s="71"/>
+      <c r="M21" s="69"/>
     </row>
     <row r="22" ht="55.2" spans="1:13">
-      <c r="A22" s="51"/>
-      <c r="B22" s="52"/>
+      <c r="A22" s="39"/>
+      <c r="B22" s="51"/>
       <c r="C22" s="43" t="s">
         <v>124</v>
       </c>
-      <c r="D22" s="53"/>
-      <c r="E22" s="53"/>
-      <c r="F22" s="53"/>
-      <c r="G22" s="53"/>
-      <c r="H22" s="53"/>
-      <c r="I22" s="53"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="53"/>
-      <c r="L22" s="53"/>
-      <c r="M22" s="72"/>
+      <c r="D22" s="52"/>
+      <c r="E22" s="52"/>
+      <c r="F22" s="52"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="52"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="52"/>
+      <c r="K22" s="52"/>
+      <c r="L22" s="52"/>
+      <c r="M22" s="70"/>
     </row>
     <row r="23" ht="27.6" spans="1:13">
-      <c r="A23" s="51"/>
-      <c r="B23" s="52"/>
+      <c r="A23" s="39"/>
+      <c r="B23" s="51"/>
       <c r="C23" s="43" t="s">
         <v>125</v>
       </c>
-      <c r="D23" s="53"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="53"/>
-      <c r="G23" s="53"/>
-      <c r="H23" s="53"/>
-      <c r="I23" s="53"/>
-      <c r="J23" s="53"/>
-      <c r="K23" s="53"/>
-      <c r="L23" s="53"/>
-      <c r="M23" s="72"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="52"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="52"/>
+      <c r="I23" s="52"/>
+      <c r="J23" s="52"/>
+      <c r="K23" s="52"/>
+      <c r="L23" s="52"/>
+      <c r="M23" s="70"/>
     </row>
     <row r="24" ht="27.6" spans="1:13">
-      <c r="A24" s="51"/>
-      <c r="B24" s="52"/>
+      <c r="A24" s="39"/>
+      <c r="B24" s="51"/>
       <c r="C24" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="D24" s="53"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="53"/>
-      <c r="G24" s="53"/>
-      <c r="H24" s="53"/>
-      <c r="I24" s="53"/>
-      <c r="J24" s="53"/>
-      <c r="K24" s="53"/>
-      <c r="L24" s="53"/>
-      <c r="M24" s="72"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="52"/>
+      <c r="L24" s="52"/>
+      <c r="M24" s="70"/>
     </row>
     <row r="25" ht="27.6" spans="1:13">
-      <c r="A25" s="51"/>
-      <c r="B25" s="52"/>
+      <c r="A25" s="39"/>
+      <c r="B25" s="51"/>
       <c r="C25" s="43" t="s">
         <v>127</v>
       </c>
-      <c r="D25" s="53"/>
-      <c r="E25" s="53"/>
-      <c r="F25" s="53"/>
-      <c r="G25" s="53"/>
-      <c r="H25" s="53"/>
-      <c r="I25" s="53"/>
-      <c r="J25" s="53"/>
-      <c r="K25" s="53"/>
-      <c r="L25" s="53"/>
-      <c r="M25" s="72"/>
+      <c r="D25" s="52"/>
+      <c r="E25" s="52"/>
+      <c r="F25" s="52"/>
+      <c r="G25" s="52"/>
+      <c r="H25" s="52"/>
+      <c r="I25" s="52"/>
+      <c r="J25" s="52"/>
+      <c r="K25" s="52"/>
+      <c r="L25" s="52"/>
+      <c r="M25" s="70"/>
     </row>
     <row r="26" ht="27.6" spans="1:13">
-      <c r="A26" s="51"/>
-      <c r="B26" s="52"/>
+      <c r="A26" s="39"/>
+      <c r="B26" s="51"/>
       <c r="C26" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="D26" s="53"/>
-      <c r="E26" s="53"/>
-      <c r="F26" s="53"/>
-      <c r="G26" s="53"/>
-      <c r="H26" s="53"/>
-      <c r="I26" s="53"/>
-      <c r="J26" s="53"/>
-      <c r="K26" s="53"/>
-      <c r="L26" s="53"/>
-      <c r="M26" s="72"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="52"/>
+      <c r="F26" s="52"/>
+      <c r="G26" s="52"/>
+      <c r="H26" s="52"/>
+      <c r="I26" s="52"/>
+      <c r="J26" s="52"/>
+      <c r="K26" s="52"/>
+      <c r="L26" s="52"/>
+      <c r="M26" s="70"/>
     </row>
     <row r="27" ht="27.6" spans="1:13">
-      <c r="A27" s="51"/>
-      <c r="B27" s="52"/>
+      <c r="A27" s="39"/>
+      <c r="B27" s="51"/>
       <c r="C27" s="43" t="s">
         <v>129</v>
       </c>
-      <c r="D27" s="53"/>
-      <c r="E27" s="53"/>
-      <c r="F27" s="53"/>
-      <c r="G27" s="53"/>
-      <c r="H27" s="53"/>
-      <c r="I27" s="53"/>
-      <c r="J27" s="53"/>
-      <c r="K27" s="53"/>
-      <c r="L27" s="53"/>
-      <c r="M27" s="72"/>
+      <c r="D27" s="52"/>
+      <c r="E27" s="52"/>
+      <c r="F27" s="52"/>
+      <c r="G27" s="52"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="52"/>
+      <c r="J27" s="52"/>
+      <c r="K27" s="52"/>
+      <c r="L27" s="52"/>
+      <c r="M27" s="70"/>
     </row>
     <row r="28" ht="55.2" spans="1:13">
-      <c r="A28" s="51"/>
-      <c r="B28" s="52"/>
+      <c r="A28" s="39"/>
+      <c r="B28" s="51"/>
       <c r="C28" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="D28" s="53"/>
-      <c r="E28" s="53"/>
-      <c r="F28" s="53"/>
-      <c r="G28" s="53"/>
-      <c r="H28" s="53"/>
-      <c r="I28" s="53"/>
-      <c r="J28" s="53"/>
-      <c r="K28" s="53"/>
-      <c r="L28" s="53"/>
-      <c r="M28" s="72"/>
+      <c r="D28" s="52"/>
+      <c r="E28" s="52"/>
+      <c r="F28" s="52"/>
+      <c r="G28" s="52"/>
+      <c r="H28" s="52"/>
+      <c r="I28" s="52"/>
+      <c r="J28" s="52"/>
+      <c r="K28" s="52"/>
+      <c r="L28" s="52"/>
+      <c r="M28" s="70"/>
     </row>
     <row r="29" ht="41.4" spans="1:13">
-      <c r="A29" s="51"/>
-      <c r="B29" s="52"/>
+      <c r="A29" s="39"/>
+      <c r="B29" s="51"/>
       <c r="C29" s="43" t="s">
         <v>131</v>
       </c>
-      <c r="D29" s="53"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="53"/>
-      <c r="G29" s="53"/>
-      <c r="H29" s="53"/>
-      <c r="I29" s="53"/>
-      <c r="J29" s="53"/>
-      <c r="K29" s="53"/>
-      <c r="L29" s="53"/>
-      <c r="M29" s="72"/>
+      <c r="D29" s="52"/>
+      <c r="E29" s="52"/>
+      <c r="F29" s="52"/>
+      <c r="G29" s="52"/>
+      <c r="H29" s="52"/>
+      <c r="I29" s="52"/>
+      <c r="J29" s="52"/>
+      <c r="K29" s="52"/>
+      <c r="L29" s="52"/>
+      <c r="M29" s="70"/>
     </row>
     <row r="30" ht="27.6" spans="1:13">
-      <c r="A30" s="51"/>
-      <c r="B30" s="52"/>
+      <c r="A30" s="39"/>
+      <c r="B30" s="51"/>
       <c r="C30" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="D30" s="53"/>
-      <c r="E30" s="53"/>
-      <c r="F30" s="53"/>
-      <c r="G30" s="53"/>
-      <c r="H30" s="53"/>
-      <c r="I30" s="53"/>
-      <c r="J30" s="53"/>
-      <c r="K30" s="53"/>
-      <c r="L30" s="53"/>
-      <c r="M30" s="72"/>
-    </row>
-    <row r="31" ht="15.6" spans="1:13">
-      <c r="A31" s="51"/>
-      <c r="B31" s="52"/>
-      <c r="C31" s="57" t="s">
+      <c r="D30" s="52"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="52"/>
+      <c r="G30" s="52"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="52"/>
+      <c r="J30" s="52"/>
+      <c r="K30" s="52"/>
+      <c r="L30" s="52"/>
+      <c r="M30" s="70"/>
+    </row>
+    <row r="31" ht="13.8" spans="1:13">
+      <c r="A31" s="39"/>
+      <c r="B31" s="51"/>
+      <c r="C31" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="D31" s="53"/>
-      <c r="E31" s="53"/>
-      <c r="F31" s="53"/>
-      <c r="G31" s="53"/>
-      <c r="H31" s="53"/>
-      <c r="I31" s="53"/>
-      <c r="J31" s="53"/>
-      <c r="K31" s="53"/>
-      <c r="L31" s="53"/>
-      <c r="M31" s="72"/>
-    </row>
-    <row r="32" ht="15.6" spans="1:13">
-      <c r="A32" s="51"/>
-      <c r="B32" s="52"/>
-      <c r="C32" s="58" t="s">
+      <c r="D31" s="52"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="52"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="52"/>
+      <c r="J31" s="52"/>
+      <c r="K31" s="52"/>
+      <c r="L31" s="52"/>
+      <c r="M31" s="70"/>
+    </row>
+    <row r="32" ht="13.8" spans="1:13">
+      <c r="A32" s="39"/>
+      <c r="B32" s="51"/>
+      <c r="C32" s="56" t="s">
         <v>103</v>
       </c>
-      <c r="D32" s="53"/>
-      <c r="E32" s="53"/>
-      <c r="F32" s="53"/>
-      <c r="G32" s="53"/>
-      <c r="H32" s="53"/>
-      <c r="I32" s="53"/>
-      <c r="J32" s="53"/>
-      <c r="K32" s="53"/>
-      <c r="L32" s="53"/>
-      <c r="M32" s="72"/>
-    </row>
-    <row r="33" ht="15.6" spans="1:13">
-      <c r="A33" s="51"/>
-      <c r="B33" s="52"/>
+      <c r="D32" s="52"/>
+      <c r="E32" s="52"/>
+      <c r="F32" s="52"/>
+      <c r="G32" s="52"/>
+      <c r="H32" s="52"/>
+      <c r="I32" s="52"/>
+      <c r="J32" s="52"/>
+      <c r="K32" s="52"/>
+      <c r="L32" s="52"/>
+      <c r="M32" s="70"/>
+    </row>
+    <row r="33" ht="13.8" spans="1:13">
+      <c r="A33" s="39"/>
+      <c r="B33" s="51"/>
       <c r="C33" s="43" t="s">
         <v>133</v>
       </c>
-      <c r="D33" s="53"/>
-      <c r="E33" s="53"/>
-      <c r="F33" s="53"/>
-      <c r="G33" s="53"/>
-      <c r="H33" s="53"/>
-      <c r="I33" s="53"/>
-      <c r="J33" s="53"/>
-      <c r="K33" s="53"/>
-      <c r="L33" s="53"/>
-      <c r="M33" s="72"/>
+      <c r="D33" s="52"/>
+      <c r="E33" s="52"/>
+      <c r="F33" s="52"/>
+      <c r="G33" s="52"/>
+      <c r="H33" s="52"/>
+      <c r="I33" s="52"/>
+      <c r="J33" s="52"/>
+      <c r="K33" s="52"/>
+      <c r="L33" s="52"/>
+      <c r="M33" s="70"/>
     </row>
     <row r="34" ht="27.6" spans="1:13">
-      <c r="A34" s="51"/>
-      <c r="B34" s="52"/>
+      <c r="A34" s="39"/>
+      <c r="B34" s="51"/>
       <c r="C34" s="43" t="s">
         <v>134</v>
       </c>
-      <c r="D34" s="53"/>
-      <c r="E34" s="53"/>
-      <c r="F34" s="53"/>
-      <c r="G34" s="53"/>
-      <c r="H34" s="53"/>
-      <c r="I34" s="53"/>
-      <c r="J34" s="53"/>
-      <c r="K34" s="53"/>
-      <c r="L34" s="53"/>
-      <c r="M34" s="72"/>
+      <c r="D34" s="52"/>
+      <c r="E34" s="52"/>
+      <c r="F34" s="52"/>
+      <c r="G34" s="52"/>
+      <c r="H34" s="52"/>
+      <c r="I34" s="52"/>
+      <c r="J34" s="52"/>
+      <c r="K34" s="52"/>
+      <c r="L34" s="52"/>
+      <c r="M34" s="70"/>
     </row>
     <row r="35" ht="28.35" spans="1:13">
-      <c r="A35" s="59"/>
-      <c r="B35" s="60"/>
-      <c r="C35" s="61" t="s">
+      <c r="A35" s="57"/>
+      <c r="B35" s="58"/>
+      <c r="C35" s="59" t="s">
         <v>135</v>
       </c>
-      <c r="D35" s="62"/>
-      <c r="E35" s="62"/>
-      <c r="F35" s="62"/>
-      <c r="G35" s="62"/>
-      <c r="H35" s="62"/>
-      <c r="I35" s="62"/>
-      <c r="J35" s="62"/>
-      <c r="K35" s="62"/>
-      <c r="L35" s="62"/>
-      <c r="M35" s="74"/>
+      <c r="D35" s="60"/>
+      <c r="E35" s="60"/>
+      <c r="F35" s="60"/>
+      <c r="G35" s="60"/>
+      <c r="H35" s="60"/>
+      <c r="I35" s="60"/>
+      <c r="J35" s="60"/>
+      <c r="K35" s="60"/>
+      <c r="L35" s="60"/>
+      <c r="M35" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -9317,7 +9264,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" sqref="A1:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="13.2" outlineLevelCol="4"/>
@@ -9954,217 +9901,217 @@
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="3:5">
+    <row r="25" ht="13.2" spans="3:5">
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="3:5">
+    <row r="26" ht="13.2" spans="3:5">
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="3:5">
+    <row r="27" ht="13.2" spans="3:5">
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="3:5">
+    <row r="28" ht="13.2" spans="3:5">
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="3:5">
+    <row r="29" ht="13.2" spans="3:5">
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="3:5">
+    <row r="30" ht="13.2" spans="3:5">
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="3:5">
+    <row r="31" ht="13.2" spans="3:5">
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="3:5">
+    <row r="32" ht="13.2" spans="3:5">
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="3:5">
+    <row r="33" ht="13.2" spans="3:5">
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="3:5">
+    <row r="34" ht="13.2" spans="3:5">
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="3:5">
+    <row r="35" ht="13.2" spans="3:5">
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="3:5">
+    <row r="36" ht="13.2" spans="3:5">
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="3:5">
+    <row r="37" ht="13.2" spans="3:5">
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="3:5">
+    <row r="38" ht="13.2" spans="3:5">
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="3:5">
+    <row r="39" ht="13.2" spans="3:5">
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="3:5">
+    <row r="40" ht="13.2" spans="3:5">
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="3:5">
+    <row r="41" ht="13.2" spans="3:5">
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="3:5">
+    <row r="42" ht="13.2" spans="3:5">
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="3:5">
+    <row r="43" ht="13.2" spans="3:5">
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="3:5">
+    <row r="44" ht="13.2" spans="3:5">
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="3:5">
+    <row r="45" ht="13.2" spans="3:5">
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="3:5">
+    <row r="46" ht="13.2" spans="3:5">
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="3:5">
+    <row r="47" ht="13.2" spans="3:5">
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="3:5">
+    <row r="48" ht="13.2" spans="3:5">
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="3:5">
+    <row r="49" ht="13.2" spans="3:5">
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="3:5">
+    <row r="50" ht="13.2" spans="3:5">
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="3:5">
+    <row r="51" ht="13.2" spans="3:5">
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="3:5">
+    <row r="52" ht="13.2" spans="3:5">
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="3:5">
+    <row r="53" ht="13.2" spans="3:5">
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="3:5">
+    <row r="54" ht="13.2" spans="3:5">
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="3:5">
+    <row r="55" ht="13.2" spans="3:5">
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="3:5">
+    <row r="56" ht="13.2" spans="3:5">
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="3:5">
+    <row r="57" ht="13.2" spans="3:5">
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="3:5">
+    <row r="58" ht="13.2" spans="3:5">
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="3:5">
+    <row r="59" ht="13.2" spans="3:5">
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="3:5">
+    <row r="60" ht="13.2" spans="3:5">
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="3:5">
+    <row r="61" ht="13.2" spans="3:5">
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="3:5">
+    <row r="62" ht="13.2" spans="3:5">
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="3:5">
+    <row r="63" ht="13.2" spans="3:5">
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="3:5">
+    <row r="64" ht="13.2" spans="3:5">
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="3:5">
+    <row r="65" ht="13.2" spans="3:5">
       <c r="C65" s="7"/>
       <c r="D65" s="7"/>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="3:5">
+    <row r="66" ht="13.2" spans="3:5">
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="3:5">
+    <row r="67" ht="13.2" spans="3:5">
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
       <c r="E67" s="7"/>

</xml_diff>